<commit_message>
$EBAY FY19/20 & Quarterly breakdown
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20393"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA75F72B-EC2A-434D-AED4-570941CC1FAA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2039089-C14B-8C49-AA38-4D5320790AE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener" sheetId="2" r:id="rId1"/>
@@ -30,12 +30,22 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="113">
   <si>
     <t>Ticker</t>
   </si>
@@ -353,6 +363,27 @@
   </si>
   <si>
     <t>Normalised to Pound Sterling (GBP) [millions]</t>
+  </si>
+  <si>
+    <t>$CVNA</t>
+  </si>
+  <si>
+    <t>Carvana</t>
+  </si>
+  <si>
+    <t>£AUTO</t>
+  </si>
+  <si>
+    <t>Auto Trader Group Plc</t>
+  </si>
+  <si>
+    <t>$CZOO</t>
+  </si>
+  <si>
+    <t>Cazoo Group Ltd</t>
+  </si>
+  <si>
+    <t>Online Auto Sales</t>
   </si>
 </sst>
 </file>
@@ -571,7 +602,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -617,15 +648,6 @@
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -639,6 +661,18 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -974,7 +1008,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1148,6 +1182,7 @@
           <cell r="G11" t="str">
             <v>Q322</v>
           </cell>
+          <cell r="H11"/>
         </row>
         <row r="12">
           <cell r="C12">
@@ -1177,7 +1212,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1250,8 +1285,34 @@
             <v>2.235768596469994</v>
           </cell>
         </row>
+        <row r="35">
+          <cell r="C35">
+            <v>2.663632811462922</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>-347.03384754378123</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>941.59419885214288</v>
+          </cell>
+        </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="20">
+          <cell r="AC20">
+            <v>1786</v>
+          </cell>
+          <cell r="AD20">
+            <v>5667</v>
+          </cell>
+          <cell r="AE20">
+            <v>13608</v>
+          </cell>
+        </row>
         <row r="27">
           <cell r="U27">
             <v>0.72815126050420165</v>
@@ -1279,7 +1340,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1567,7 +1628,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1584,9 +1645,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1595,55 +1656,55 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1873CD5B-C727-4CC0-ACC4-210B76523995}">
-  <dimension ref="A1:AI38"/>
+  <dimension ref="A1:AI44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="K30" sqref="K30"/>
+      <selection pane="bottomRight" activeCell="S26" sqref="R26:S26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
-    <col min="6" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="19" width="9.42578125" style="5" customWidth="1"/>
-    <col min="20" max="23" width="9.42578125" style="26" customWidth="1"/>
-    <col min="24" max="24" width="9.140625" style="1"/>
-    <col min="25" max="28" width="9.140625" style="5"/>
-    <col min="29" max="29" width="9.140625" style="1"/>
-    <col min="30" max="31" width="9.140625" style="5"/>
-    <col min="32" max="32" width="16.85546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.140625" style="1"/>
-    <col min="34" max="34" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="5" width="9.1640625" style="5"/>
+    <col min="6" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="9.1640625" style="5"/>
+    <col min="12" max="12" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="19" width="9.5" style="5" customWidth="1"/>
+    <col min="20" max="23" width="9.5" style="23" customWidth="1"/>
+    <col min="24" max="24" width="9.1640625" style="1"/>
+    <col min="25" max="28" width="9.1640625" style="5"/>
+    <col min="29" max="29" width="9.1640625" style="1"/>
+    <col min="30" max="31" width="9.1640625" style="5"/>
+    <col min="32" max="32" width="16.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.1640625" style="1"/>
+    <col min="34" max="34" width="16.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="24.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="23" t="s">
+    <row r="1" spans="1:35" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="S1" s="23" t="s">
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="S1" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
       <c r="X1" s="5"/>
     </row>
-    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -1738,29 +1799,29 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.15">
       <c r="F3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="28"/>
-      <c r="U3" s="28"/>
-      <c r="V3" s="28"/>
-      <c r="W3" s="28"/>
+      <c r="S3" s="22"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="25"/>
+      <c r="W3" s="25"/>
       <c r="AI3" s="5"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.15">
       <c r="F4" s="16"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
-      <c r="S4" s="25"/>
-      <c r="T4" s="28"/>
-      <c r="U4" s="28"/>
-      <c r="V4" s="28"/>
-      <c r="W4" s="28"/>
+      <c r="S4" s="22"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="25"/>
+      <c r="W4" s="25"/>
       <c r="AI4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
         <v>32</v>
       </c>
@@ -1774,7 +1835,7 @@
         <v>17</v>
       </c>
       <c r="F5" s="16">
-        <f>[1]Main!$C$6*F37</f>
+        <f>[1]Main!$C$6*F43</f>
         <v>159.1525</v>
       </c>
       <c r="G5" s="19">
@@ -1782,15 +1843,15 @@
         <v>68.916813000000005</v>
       </c>
       <c r="H5" s="17">
-        <f>[1]Main!$C$8*F37</f>
+        <f>[1]Main!$C$8*F43</f>
         <v>10968.283080982501</v>
       </c>
       <c r="I5" s="17">
-        <f>[1]Main!$C$11*F37</f>
+        <f>[1]Main!$C$11*F43</f>
         <v>538.24670000000003</v>
       </c>
       <c r="J5" s="17">
-        <f>[1]Main!$C$12*F37</f>
+        <f>[1]Main!$C$12*F43</f>
         <v>10430.036380982501</v>
       </c>
       <c r="K5" s="5" t="str">
@@ -1801,11 +1862,11 @@
         <f>[1]Main!$D$28</f>
         <v>44901</v>
       </c>
-      <c r="M5" s="24">
+      <c r="M5" s="21">
         <f>[1]Main!$C$33</f>
         <v>19.311919490429393</v>
       </c>
-      <c r="N5" s="24">
+      <c r="N5" s="21">
         <f>[1]Main!$C$34</f>
         <v>11.112137929461445</v>
       </c>
@@ -1813,17 +1874,17 @@
       <c r="P5" s="8"/>
       <c r="Q5" s="8"/>
       <c r="R5" s="8"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="28">
-        <f>'[1]Financial Model'!$AH$21*F37</f>
+      <c r="S5" s="22"/>
+      <c r="T5" s="25">
+        <f>'[1]Financial Model'!$AH$21*F43</f>
         <v>-254.69877999999997</v>
       </c>
-      <c r="U5" s="28">
-        <f>'[1]Financial Model'!$AG$15*F37</f>
+      <c r="U5" s="25">
+        <f>'[1]Financial Model'!$AG$15*F43</f>
         <v>-173.72231999999997</v>
       </c>
-      <c r="V5" s="28"/>
-      <c r="W5" s="28"/>
+      <c r="V5" s="25"/>
+      <c r="W5" s="25"/>
       <c r="Y5" s="18">
         <f>'[1]Financial Model'!$X$29</f>
         <v>0.70928999538958049</v>
@@ -1859,7 +1920,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B6" s="7" t="s">
         <v>80</v>
       </c>
@@ -1873,7 +1934,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="16">
-        <f>[2]Main!$C$6*F37</f>
+        <f>[2]Main!$C$6*F43</f>
         <v>3.3365999999999993</v>
       </c>
       <c r="G6" s="17">
@@ -1881,15 +1942,15 @@
         <v>58.801357000000003</v>
       </c>
       <c r="H6" s="17">
-        <f>[2]Main!$C$8*F37</f>
+        <f>[2]Main!$C$8*F43</f>
         <v>196.19660776619997</v>
       </c>
       <c r="I6" s="17">
-        <f>[2]Main!$C$11*F37</f>
+        <f>[2]Main!$C$11*F43</f>
         <v>13.289129999999998</v>
       </c>
       <c r="J6" s="17">
-        <f>[2]Main!$C$12*F37</f>
+        <f>[2]Main!$C$12*F43</f>
         <v>182.90747776619997</v>
       </c>
       <c r="K6" s="5" t="str">
@@ -1900,20 +1961,20 @@
         <f>[2]Main!$D$28</f>
         <v>42705</v>
       </c>
-      <c r="M6" s="24">
+      <c r="M6" s="21">
         <f>[2]Main!$C$34</f>
         <v>26.782399177430296</v>
       </c>
-      <c r="N6" s="24"/>
-      <c r="O6" s="24"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
       <c r="R6" s="8"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="28"/>
-      <c r="U6" s="28"/>
-      <c r="V6" s="28"/>
-      <c r="W6" s="28"/>
+      <c r="S6" s="22"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="25"/>
+      <c r="W6" s="25"/>
       <c r="Y6" s="18">
         <f>'[2]Financial Model'!$J$28</f>
         <v>0.68957308000457829</v>
@@ -1949,22 +2010,22 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.15">
       <c r="F7" s="16"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
-      <c r="N7" s="24"/>
-      <c r="O7" s="24"/>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="24"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="28"/>
-      <c r="U7" s="28"/>
-      <c r="V7" s="28"/>
-      <c r="W7" s="28"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="S7" s="22"/>
+      <c r="T7" s="25"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="25"/>
+      <c r="W7" s="25"/>
       <c r="AI7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B8" s="7" t="s">
         <v>14</v>
       </c>
@@ -1978,7 +2039,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="16">
-        <f>[3]Main!$C$6*$F$37</f>
+        <f>[3]Main!$C$6*$F$43</f>
         <v>40.686599999999999</v>
       </c>
       <c r="G8" s="17">
@@ -1986,15 +2047,15 @@
         <v>183.692564</v>
       </c>
       <c r="H8" s="17">
-        <f>[3]Main!$C$8*$F$37</f>
+        <f>[3]Main!$C$8*$F$43</f>
         <v>7473.8258744424002</v>
       </c>
       <c r="I8" s="17">
-        <f>[3]Main!$C$11*F37</f>
+        <f>[3]Main!$C$11*F43</f>
         <v>2653.2759399999995</v>
       </c>
       <c r="J8" s="17">
-        <f>[3]Main!$C$12*F37</f>
+        <f>[3]Main!$C$12*F43</f>
         <v>4820.5499344424006</v>
       </c>
       <c r="K8" s="5" t="str">
@@ -2005,42 +2066,42 @@
         <f>[3]Main!$D$28</f>
         <v>37926</v>
       </c>
-      <c r="M8" s="24">
+      <c r="M8" s="21">
         <f>[3]Main!$C$33</f>
         <v>0.85506649460900186</v>
       </c>
-      <c r="N8" s="24">
+      <c r="N8" s="21">
         <f>[3]Main!$C$34</f>
         <v>2.4707454311946444</v>
       </c>
-      <c r="O8" s="24">
+      <c r="O8" s="21">
         <f>[3]Main!$C$35</f>
         <v>1.5936084043780052</v>
       </c>
-      <c r="P8" s="24">
+      <c r="P8" s="21">
         <f>[3]Main!$C$36</f>
         <v>-6.7618910307413636</v>
       </c>
-      <c r="Q8" s="24">
+      <c r="Q8" s="21">
         <f>[3]Main!$C$37</f>
         <v>-4.4061966235825452</v>
       </c>
       <c r="R8" s="8"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="28">
-        <f>'[3]Financial Model'!$AB$17*$F$37</f>
+      <c r="S8" s="22"/>
+      <c r="T8" s="25">
+        <f>'[3]Financial Model'!$AB$17*$F$43</f>
         <v>-788.41700000000003</v>
       </c>
-      <c r="U8" s="28">
-        <f>'[3]Financial Model'!$AA$17*$F$37</f>
+      <c r="U8" s="25">
+        <f>'[3]Financial Model'!$AA$17*$F$43</f>
         <v>-407.51256999999981</v>
       </c>
-      <c r="V8" s="28">
-        <f>'[3]Financial Model'!$Z$17*$F$37</f>
+      <c r="V8" s="25">
+        <f>'[3]Financial Model'!$Z$17*$F$43</f>
         <v>-254.86228999999994</v>
       </c>
-      <c r="W8" s="28">
-        <f>'[3]Financial Model'!$Y$17*F37</f>
+      <c r="W8" s="25">
+        <f>'[3]Financial Model'!$Y$17*F43</f>
         <v>-101.21767</v>
       </c>
       <c r="Y8" s="18">
@@ -2078,7 +2139,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B9" s="7"/>
       <c r="F9" s="16"/>
       <c r="G9" s="17"/>
@@ -2087,23 +2148,23 @@
       <c r="J9" s="17"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
       <c r="R9" s="8"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="28"/>
-      <c r="U9" s="28"/>
-      <c r="V9" s="28"/>
-      <c r="W9" s="28"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="25"/>
+      <c r="U9" s="25"/>
+      <c r="V9" s="25"/>
+      <c r="W9" s="25"/>
       <c r="Y9" s="18"/>
       <c r="Z9" s="18"/>
       <c r="AA9" s="18"/>
       <c r="AB9" s="18"/>
       <c r="AI9" s="5"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>34</v>
       </c>
@@ -2113,15 +2174,15 @@
       <c r="E10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N10" s="24"/>
-      <c r="O10" s="24"/>
-      <c r="P10" s="24"/>
-      <c r="Q10" s="24"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="28"/>
-      <c r="U10" s="28"/>
-      <c r="V10" s="28"/>
-      <c r="W10" s="28"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="S10" s="22"/>
+      <c r="T10" s="25"/>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25"/>
+      <c r="W10" s="25"/>
       <c r="AH10" s="5" t="s">
         <v>15</v>
       </c>
@@ -2129,7 +2190,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2139,11 +2200,11 @@
       <c r="E11" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S11" s="25"/>
-      <c r="T11" s="28"/>
-      <c r="U11" s="28"/>
-      <c r="V11" s="28"/>
-      <c r="W11" s="28"/>
+      <c r="S11" s="22"/>
+      <c r="T11" s="25"/>
+      <c r="U11" s="25"/>
+      <c r="V11" s="25"/>
+      <c r="W11" s="25"/>
       <c r="AH11" s="5" t="s">
         <v>15</v>
       </c>
@@ -2151,7 +2212,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
@@ -2192,44 +2253,44 @@
         <f>[4]Main!$D$27</f>
         <v>44881</v>
       </c>
-      <c r="M12" s="24">
+      <c r="M12" s="21">
         <f>[4]Main!$C$34</f>
         <v>5.5155555555555553</v>
       </c>
-      <c r="N12" s="24">
+      <c r="N12" s="21">
         <f>[4]Main!$C$33</f>
         <v>3.9008320493066257</v>
       </c>
-      <c r="O12" s="24">
+      <c r="O12" s="21">
         <f>[4]Main!$C$35</f>
         <v>4.2752542372881353</v>
       </c>
-      <c r="P12" s="24">
+      <c r="P12" s="21">
         <f>[4]Main!$C$32</f>
         <v>29.901259842519682</v>
       </c>
-      <c r="Q12" s="24">
+      <c r="Q12" s="21">
         <f>[4]Main!$C$36</f>
         <v>32.771338582677167</v>
       </c>
       <c r="R12" s="20"/>
-      <c r="S12" s="28">
+      <c r="S12" s="25">
         <f>'[4]Financial Model'!$V$13</f>
         <v>254</v>
       </c>
-      <c r="T12" s="28">
+      <c r="T12" s="25">
         <f>'[4]Financial Model'!$U$13</f>
         <v>285</v>
       </c>
-      <c r="U12" s="28">
+      <c r="U12" s="25">
         <f>'[4]Financial Model'!$T$13</f>
         <v>310</v>
       </c>
-      <c r="V12" s="28">
+      <c r="V12" s="25">
         <f>'[4]Financial Model'!$S$13</f>
         <v>266</v>
       </c>
-      <c r="W12" s="28">
+      <c r="W12" s="25">
         <f>'[4]Financial Model'!$R$13</f>
         <v>295</v>
       </c>
@@ -2268,17 +2329,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B13" s="7"/>
       <c r="F13" s="16"/>
       <c r="AI13" s="5"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
         <v>76</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>77</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>17</v>
       </c>
       <c r="AD14" s="5">
         <v>2002</v>
@@ -2297,7 +2364,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2314,7 +2381,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
         <v>63</v>
       </c>
@@ -2331,7 +2398,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
@@ -2348,7 +2415,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B21" s="7" t="s">
         <v>57</v>
       </c>
@@ -2362,7 +2429,7 @@
         <v>17</v>
       </c>
       <c r="F21" s="17">
-        <f>[5]Main!$C$6*F37</f>
+        <f>[5]Main!$C$6*F43</f>
         <v>21.712799999999998</v>
       </c>
       <c r="G21" s="17">
@@ -2370,15 +2437,15 @@
         <v>597.779</v>
       </c>
       <c r="H21" s="17">
-        <f>[5]Main!$C$8*F37</f>
+        <f>[5]Main!$C$8*F43</f>
         <v>12979.455871199998</v>
       </c>
       <c r="I21" s="17">
-        <f>[5]Main!$C$11*F37</f>
+        <f>[5]Main!$C$11*F43</f>
         <v>1687.26052</v>
       </c>
       <c r="J21" s="17">
-        <f>[5]Main!$C$12*F37</f>
+        <f>[5]Main!$C$12*F43</f>
         <v>11292.1953512</v>
       </c>
       <c r="K21" s="5" t="str">
@@ -2424,7 +2491,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B23" s="7" t="s">
         <v>82</v>
       </c>
@@ -2438,7 +2505,7 @@
         <v>17</v>
       </c>
       <c r="F23" s="16">
-        <f>[6]Main!$C$6*F37</f>
+        <f>[6]Main!$C$6*F43</f>
         <v>33.8474</v>
       </c>
       <c r="G23" s="19">
@@ -2446,15 +2513,15 @@
         <v>542.659087</v>
       </c>
       <c r="H23" s="17">
-        <f>[6]Main!$C$8*F37</f>
+        <f>[6]Main!$C$8*F43</f>
         <v>18367.5991813238</v>
       </c>
       <c r="I23" s="17">
-        <f>[6]Main!$C$11*F37</f>
+        <f>[6]Main!$C$11*F43</f>
         <v>-3515.0499999999997</v>
       </c>
       <c r="J23" s="17">
-        <f>[6]Main!$C$12*F37</f>
+        <f>[6]Main!$C$12*F43</f>
         <v>21882.649181323799</v>
       </c>
       <c r="K23" s="5" t="str">
@@ -2465,23 +2532,41 @@
         <f>[6]Main!$D$28</f>
         <v>37561</v>
       </c>
-      <c r="M23" s="24">
+      <c r="M23" s="21">
         <f>[6]Main!$C$33</f>
         <v>4.5599912565134968</v>
       </c>
-      <c r="N23" s="24">
+      <c r="N23" s="21">
         <f>[6]Main!$C$34</f>
         <v>2.235768596469994</v>
       </c>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
+      <c r="O23" s="21">
+        <f>[6]Main!$C$35</f>
+        <v>2.663632811462922</v>
+      </c>
+      <c r="P23" s="21">
+        <f>[6]Main!$C$36</f>
+        <v>-347.03384754378123</v>
+      </c>
+      <c r="Q23" s="21">
+        <f>[6]Main!$C$37</f>
+        <v>941.59419885214288</v>
+      </c>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27"/>
+      <c r="T23" s="29">
+        <f>'[6]Financial Model'!$AE$20*F43</f>
+        <v>11294.64</v>
+      </c>
+      <c r="U23" s="29">
+        <f>'[6]Financial Model'!$AD$20*F43</f>
+        <v>4703.6099999999997</v>
+      </c>
+      <c r="V23" s="29">
+        <f>'[6]Financial Model'!$AC$20*F43</f>
+        <v>1482.3799999999999</v>
+      </c>
+      <c r="W23" s="24"/>
       <c r="Y23" s="18">
         <f>'[6]Financial Model'!$U$27</f>
         <v>0.72815126050420165</v>
@@ -2517,7 +2602,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -2532,7 +2617,7 @@
       </c>
       <c r="AI24" s="5"/>
     </row>
-    <row r="25" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>87</v>
       </c>
@@ -2550,7 +2635,7 @@
       </c>
       <c r="AI25" s="5"/>
     </row>
-    <row r="26" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>89</v>
       </c>
@@ -2568,7 +2653,7 @@
       </c>
       <c r="AI26" s="5"/>
     </row>
-    <row r="27" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>91</v>
       </c>
@@ -2583,7 +2668,7 @@
       </c>
       <c r="AI27" s="5"/>
     </row>
-    <row r="28" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
         <v>93</v>
       </c>
@@ -2595,7 +2680,7 @@
       </c>
       <c r="AI28" s="5"/>
     </row>
-    <row r="31" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>66</v>
       </c>
@@ -2612,7 +2697,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:35" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
         <v>68</v>
       </c>
@@ -2626,42 +2711,90 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E36" s="21" t="s">
+    <row r="35" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B35" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="AH35" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI35" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B36" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH36" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI36" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="37" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B37" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="AH37" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AI37" s="5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="42" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="E42" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="9" t="s">
+      <c r="F42" s="27"/>
+      <c r="G42" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E37" s="10" t="s">
+    <row r="43" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="E43" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F37" s="11">
+      <c r="F43" s="11">
         <v>0.83</v>
       </c>
-      <c r="G37" s="12">
-        <f>1/F37</f>
+      <c r="G43" s="12">
+        <f>1/F43</f>
         <v>1.2048192771084338</v>
       </c>
     </row>
-    <row r="38" spans="5:7" x14ac:dyDescent="0.2">
-      <c r="E38" s="13" t="s">
+    <row r="44" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="E44" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F38" s="14">
+      <c r="F44" s="14">
         <v>0.87</v>
       </c>
-      <c r="G38" s="15">
-        <f>1/F38</f>
+      <c r="G44" s="15">
+        <f>1/F44</f>
         <v>1.1494252873563218</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E42:F42"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="S1:W1"/>
   </mergeCells>
@@ -2686,24 +2819,24 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.140625" style="1"/>
+    <col min="4" max="8" width="9.1640625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2736,7 +2869,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -2762,11 +2895,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add UK software/tech to list
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391F5142-8C2A-864F-9ABE-8BAE54FFD8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEF2797-268F-3E47-839B-0F7AAEACBB30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="133">
   <si>
     <t>Ticker</t>
   </si>
@@ -386,9 +386,6 @@
     <t>Online Auto Sales</t>
   </si>
   <si>
-    <t>E-Commerce, Logistics</t>
-  </si>
-  <si>
     <t>£TRST</t>
   </si>
   <si>
@@ -402,6 +399,51 @@
   </si>
   <si>
     <t>Copenhagen, Denmark</t>
+  </si>
+  <si>
+    <t>E-Commerce, Logistics, Cloud</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>$SPOT</t>
+  </si>
+  <si>
+    <t>$NFLX</t>
+  </si>
+  <si>
+    <t>Spotify Technology S.A.</t>
+  </si>
+  <si>
+    <t>Netflix, Inc.</t>
+  </si>
+  <si>
+    <t>Movies</t>
+  </si>
+  <si>
+    <t>Music</t>
+  </si>
+  <si>
+    <t>SaaS Streaming</t>
+  </si>
+  <si>
+    <t>Computacenter Plc</t>
+  </si>
+  <si>
+    <t>Idox Plc</t>
+  </si>
+  <si>
+    <t>Softcat Plc</t>
+  </si>
+  <si>
+    <t>£IDOX</t>
+  </si>
+  <si>
+    <t>£CCC</t>
+  </si>
+  <si>
+    <t>£SCT</t>
   </si>
 </sst>
 </file>
@@ -1671,13 +1713,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1873CD5B-C727-4CC0-ACC4-210B76523995}">
-  <dimension ref="A1:AI46"/>
+  <dimension ref="A1:AI55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AD41" sqref="AD41"/>
+      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1850,24 +1892,24 @@
         <v>17</v>
       </c>
       <c r="F5" s="16">
-        <f>[1]Main!$C$6*F45</f>
-        <v>159.1525</v>
+        <f>[1]Main!$C$6*F54</f>
+        <v>157.23499999999999</v>
       </c>
       <c r="G5" s="19">
         <f>[1]Main!$C$7</f>
         <v>68.916813000000005</v>
       </c>
       <c r="H5" s="17">
-        <f>[1]Main!$C$8*F45</f>
-        <v>10968.283080982501</v>
+        <f>[1]Main!$C$8*F54</f>
+        <v>10836.135092054999</v>
       </c>
       <c r="I5" s="17">
-        <f>[1]Main!$C$11*F45</f>
-        <v>538.24670000000003</v>
+        <f>[1]Main!$C$11*F54</f>
+        <v>531.76179999999999</v>
       </c>
       <c r="J5" s="17">
-        <f>[1]Main!$C$12*F45</f>
-        <v>10430.036380982501</v>
+        <f>[1]Main!$C$12*F54</f>
+        <v>10304.373292055001</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>[1]Main!$C$28</f>
@@ -1891,12 +1933,12 @@
       <c r="R5" s="8"/>
       <c r="S5" s="22"/>
       <c r="T5" s="24">
-        <f>'[1]Financial Model'!$AH$21*F45</f>
-        <v>-254.69877999999997</v>
+        <f>'[1]Financial Model'!$AH$21*F54</f>
+        <v>-251.63011999999998</v>
       </c>
       <c r="U5" s="24">
-        <f>'[1]Financial Model'!$AG$15*F45</f>
-        <v>-173.72231999999997</v>
+        <f>'[1]Financial Model'!$AG$15*F54</f>
+        <v>-171.62927999999997</v>
       </c>
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
@@ -1949,24 +1991,24 @@
         <v>17</v>
       </c>
       <c r="F6" s="16">
-        <f>[2]Main!$C$6*F45</f>
-        <v>3.3365999999999993</v>
+        <f>[2]Main!$C$6*F54</f>
+        <v>3.2963999999999993</v>
       </c>
       <c r="G6" s="17">
         <f>[2]Main!$C$7</f>
         <v>58.801357000000003</v>
       </c>
       <c r="H6" s="17">
-        <f>[2]Main!$C$8*F45</f>
-        <v>196.19660776619997</v>
+        <f>[2]Main!$C$8*F54</f>
+        <v>193.83279321479998</v>
       </c>
       <c r="I6" s="17">
-        <f>[2]Main!$C$11*F45</f>
-        <v>13.289129999999998</v>
+        <f>[2]Main!$C$11*F54</f>
+        <v>13.129019999999999</v>
       </c>
       <c r="J6" s="17">
-        <f>[2]Main!$C$12*F45</f>
-        <v>182.90747776619997</v>
+        <f>[2]Main!$C$12*F54</f>
+        <v>180.70377321479998</v>
       </c>
       <c r="K6" s="5" t="str">
         <f>[2]Main!$C$28</f>
@@ -2054,24 +2096,24 @@
         <v>17</v>
       </c>
       <c r="F8" s="16">
-        <f>[3]Main!$C$6*$F$45</f>
-        <v>40.686599999999999</v>
+        <f>[3]Main!$C$6*$F$54</f>
+        <v>40.196399999999997</v>
       </c>
       <c r="G8" s="17">
         <f>[3]Main!$C$7</f>
         <v>183.692564</v>
       </c>
       <c r="H8" s="17">
-        <f>[3]Main!$C$8*$F$45</f>
-        <v>7473.8258744424002</v>
+        <f>[3]Main!$C$8*$F$54</f>
+        <v>7383.7797795695997</v>
       </c>
       <c r="I8" s="17">
-        <f>[3]Main!$C$11*F45</f>
-        <v>2653.2759399999995</v>
+        <f>[3]Main!$C$11*F54</f>
+        <v>2621.3087599999999</v>
       </c>
       <c r="J8" s="17">
-        <f>[3]Main!$C$12*F45</f>
-        <v>4820.5499344424006</v>
+        <f>[3]Main!$C$12*F54</f>
+        <v>4762.4710195695998</v>
       </c>
       <c r="K8" s="5" t="str">
         <f>[3]Main!$C$28</f>
@@ -2104,20 +2146,20 @@
       <c r="R8" s="8"/>
       <c r="S8" s="22"/>
       <c r="T8" s="24">
-        <f>'[3]Financial Model'!$AB$17*$F$45</f>
-        <v>-788.41700000000003</v>
+        <f>'[3]Financial Model'!$AB$17*$F$54</f>
+        <v>-778.91800000000001</v>
       </c>
       <c r="U8" s="24">
-        <f>'[3]Financial Model'!$AA$17*$F$45</f>
-        <v>-407.51256999999981</v>
+        <f>'[3]Financial Model'!$AA$17*$F$54</f>
+        <v>-402.60277999999983</v>
       </c>
       <c r="V8" s="24">
-        <f>'[3]Financial Model'!$Z$17*$F$45</f>
-        <v>-254.86228999999994</v>
+        <f>'[3]Financial Model'!$Z$17*$F$54</f>
+        <v>-251.79165999999992</v>
       </c>
       <c r="W8" s="24">
-        <f>'[3]Financial Model'!$Y$17*F45</f>
-        <v>-101.21767</v>
+        <f>'[3]Financial Model'!$Y$17*F54</f>
+        <v>-99.998180000000005</v>
       </c>
       <c r="Y8" s="18">
         <f>'[3]Financial Model'!$U$24</f>
@@ -2444,24 +2486,24 @@
         <v>17</v>
       </c>
       <c r="F21" s="17">
-        <f>[5]Main!$C$6*F45</f>
-        <v>21.712799999999998</v>
+        <f>[5]Main!$C$6*F54</f>
+        <v>21.4512</v>
       </c>
       <c r="G21" s="17">
         <f>[5]Main!$C$7</f>
         <v>597.779</v>
       </c>
       <c r="H21" s="17">
-        <f>[5]Main!$C$8*F45</f>
-        <v>12979.455871199998</v>
+        <f>[5]Main!$C$8*F54</f>
+        <v>12823.076884799999</v>
       </c>
       <c r="I21" s="17">
-        <f>[5]Main!$C$11*F45</f>
-        <v>1687.26052</v>
+        <f>[5]Main!$C$11*F54</f>
+        <v>1666.93208</v>
       </c>
       <c r="J21" s="17">
-        <f>[5]Main!$C$12*F45</f>
-        <v>11292.1953512</v>
+        <f>[5]Main!$C$12*F54</f>
+        <v>11156.1448048</v>
       </c>
       <c r="K21" s="5" t="str">
         <f>[5]Main!$G$11</f>
@@ -2520,24 +2562,24 @@
         <v>17</v>
       </c>
       <c r="F23" s="16">
-        <f>[6]Main!$C$6*F45</f>
-        <v>33.8474</v>
+        <f>[6]Main!$C$6*F54</f>
+        <v>33.439599999999999</v>
       </c>
       <c r="G23" s="19">
         <f>[6]Main!$C$7</f>
         <v>542.659087</v>
       </c>
       <c r="H23" s="17">
-        <f>[6]Main!$C$8*F45</f>
-        <v>18367.5991813238</v>
+        <f>[6]Main!$C$8*F54</f>
+        <v>18146.302805645199</v>
       </c>
       <c r="I23" s="17">
-        <f>[6]Main!$C$11*F45</f>
-        <v>-3515.0499999999997</v>
+        <f>[6]Main!$C$11*F54</f>
+        <v>-3472.7</v>
       </c>
       <c r="J23" s="17">
-        <f>[6]Main!$C$12*F45</f>
-        <v>21882.649181323799</v>
+        <f>[6]Main!$C$12*F54</f>
+        <v>21619.002805645199</v>
       </c>
       <c r="K23" s="5" t="str">
         <f>[6]Main!$C$28</f>
@@ -2570,20 +2612,20 @@
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
       <c r="T23" s="25">
-        <f>'[6]Financial Model'!$AE$20*F45</f>
-        <v>-1118.01</v>
+        <f>'[6]Financial Model'!$AE$20*F54</f>
+        <v>-1104.54</v>
       </c>
       <c r="U23" s="25">
-        <f>'[6]Financial Model'!$AD$20*F45</f>
-        <v>6030.78</v>
+        <f>'[6]Financial Model'!$AD$20*F54</f>
+        <v>5958.12</v>
       </c>
       <c r="V23" s="25">
-        <f>'[6]Financial Model'!$AC$20*F45</f>
-        <v>1431.75</v>
+        <f>'[6]Financial Model'!$AC$20*F54</f>
+        <v>1414.5</v>
       </c>
       <c r="W23" s="25">
-        <f>'[6]Financial Model'!$AC$20*G45</f>
-        <v>2078.3132530120483</v>
+        <f>'[6]Financial Model'!$AC$20*G54</f>
+        <v>2103.6585365853657</v>
       </c>
       <c r="Y23" s="18">
         <f>'[6]Financial Model'!$U$27</f>
@@ -2634,7 +2676,7 @@
         <v>84</v>
       </c>
       <c r="AI24" s="5" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
     </row>
     <row r="25" spans="2:35" x14ac:dyDescent="0.15">
@@ -2758,6 +2800,9 @@
       <c r="E36" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="Q36" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="AH36" s="5" t="s">
         <v>84</v>
       </c>
@@ -2784,10 +2829,10 @@
     </row>
     <row r="40" spans="2:35" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C40" s="6" t="s">
         <v>114</v>
-      </c>
-      <c r="C40" s="6" t="s">
-        <v>115</v>
       </c>
       <c r="D40" s="5" t="s">
         <v>31</v>
@@ -2812,51 +2857,163 @@
         <v>2021</v>
       </c>
       <c r="AF40" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AH40" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AI40" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="41" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="G41" s="19"/>
+      <c r="H41" s="17"/>
+      <c r="AI41" s="5"/>
+    </row>
+    <row r="42" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="G42" s="19"/>
+      <c r="H42" s="17"/>
+      <c r="AI42" s="5"/>
+    </row>
+    <row r="43" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F43" s="16">
+        <f>332.82*F54</f>
+        <v>272.91239999999999</v>
+      </c>
+      <c r="G43" s="19">
+        <v>445.02</v>
+      </c>
+      <c r="H43" s="17">
+        <f>G43*F43</f>
+        <v>121451.47624799999</v>
+      </c>
+      <c r="AH43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI43" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="2:35" x14ac:dyDescent="0.15">
-      <c r="E44" s="26" t="s">
+      <c r="B44" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>122</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F44" s="16">
+        <f>92.06*F54</f>
+        <v>75.489199999999997</v>
+      </c>
+      <c r="G44" s="19">
+        <v>193.13</v>
+      </c>
+      <c r="H44" s="17">
+        <f>G44*F44</f>
+        <v>14579.229195999998</v>
+      </c>
+      <c r="AH44" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="AI44" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="G45" s="19"/>
+      <c r="H45" s="17"/>
+      <c r="AI45" s="5"/>
+    </row>
+    <row r="46" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B46" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G46" s="19"/>
+      <c r="H46" s="17"/>
+      <c r="AI46" s="5"/>
+    </row>
+    <row r="47" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="G47" s="19"/>
+      <c r="H47" s="17"/>
+      <c r="AI47" s="5"/>
+    </row>
+    <row r="48" spans="2:35" x14ac:dyDescent="0.15">
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="19"/>
+      <c r="H48" s="17"/>
+      <c r="AI48" s="5"/>
+    </row>
+    <row r="49" spans="5:35" x14ac:dyDescent="0.15">
+      <c r="G49" s="19"/>
+      <c r="H49" s="17"/>
+      <c r="AI49" s="5"/>
+    </row>
+    <row r="53" spans="5:35" x14ac:dyDescent="0.15">
+      <c r="E53" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="F44" s="27"/>
-      <c r="G44" s="9" t="s">
+      <c r="F53" s="27"/>
+      <c r="G53" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="45" spans="2:35" x14ac:dyDescent="0.15">
-      <c r="E45" s="10" t="s">
+    <row r="54" spans="5:35" x14ac:dyDescent="0.15">
+      <c r="E54" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F45" s="11">
-        <v>0.83</v>
-      </c>
-      <c r="G45" s="12">
-        <f>1/F45</f>
-        <v>1.2048192771084338</v>
-      </c>
-    </row>
-    <row r="46" spans="2:35" x14ac:dyDescent="0.15">
-      <c r="E46" s="13" t="s">
+      <c r="F54" s="11">
+        <v>0.82</v>
+      </c>
+      <c r="G54" s="12">
+        <f>1/F54</f>
+        <v>1.2195121951219512</v>
+      </c>
+    </row>
+    <row r="55" spans="5:35" x14ac:dyDescent="0.15">
+      <c r="E55" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F46" s="14">
+      <c r="F55" s="14">
         <v>0.87</v>
       </c>
-      <c r="G46" s="15">
-        <f>1/F46</f>
+      <c r="G55" s="15">
+        <f>1/F55</f>
         <v>1.1494252873563218</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E53:F53"/>
     <mergeCell ref="F1:J1"/>
     <mergeCell ref="S1:W1"/>
   </mergeCells>

</xml_diff>

<commit_message>
$SHOP Q322 income & balance sheet
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0FFFB00-7598-43DE-8743-C8C97AFE34D1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BA1AAA-6189-4F1A-ADBE-92E53ED2C510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
@@ -1607,22 +1607,22 @@
         </row>
         <row r="7">
           <cell r="C7">
-            <v>1190</v>
+            <v>1269.4252260000001</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>62986.7</v>
+            <v>67190.677212180002</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>0</v>
+            <v>4028.7079999999996</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>62986.7</v>
+            <v>63161.969212180004</v>
           </cell>
         </row>
         <row r="23">
@@ -1640,8 +1640,27 @@
             <v>2015</v>
           </cell>
         </row>
+        <row r="28">
+          <cell r="C28" t="str">
+            <v>Q322</v>
+          </cell>
+          <cell r="D28">
+            <v>46661</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="C33">
+            <v>7.729278198315245</v>
+          </cell>
+        </row>
       </sheetData>
-      <sheetData sheetId="1"/>
+      <sheetData sheetId="1">
+        <row r="29">
+          <cell r="U29">
+            <v>0.48479871175523354</v>
+          </cell>
+        </row>
+      </sheetData>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1967,10 +1986,10 @@
   <dimension ref="A1:AM55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24"/>
+      <selection pane="bottomRight" activeCell="AC22" sqref="AC22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2937,19 +2956,35 @@
       </c>
       <c r="G22" s="17">
         <f>[8]Main!$C$7</f>
-        <v>1190</v>
+        <v>1269.4252260000001</v>
       </c>
       <c r="H22" s="17">
         <f>[8]Main!$C$8*F54</f>
-        <v>51019.226999999999</v>
+        <v>54424.448541865808</v>
       </c>
       <c r="I22" s="17">
         <f>[8]Main!$C$11*F54</f>
-        <v>0</v>
+        <v>3263.2534799999999</v>
       </c>
       <c r="J22" s="17">
         <f>[8]Main!$C$12*F54</f>
-        <v>51019.226999999999</v>
+        <v>51161.195061865808</v>
+      </c>
+      <c r="K22" s="5" t="str">
+        <f>[8]Main!$C$28</f>
+        <v>Q322</v>
+      </c>
+      <c r="L22" s="8">
+        <f>[8]Main!$D$28</f>
+        <v>46661</v>
+      </c>
+      <c r="Q22" s="21">
+        <f>[8]Main!$C$33</f>
+        <v>7.729278198315245</v>
+      </c>
+      <c r="AC22" s="18">
+        <f>'[8]Financial Model'!$U$29</f>
+        <v>0.48479871175523354</v>
       </c>
       <c r="AH22" s="5">
         <f>[8]Main!$C$24</f>

</xml_diff>

<commit_message>
More work to $SHOP
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BA1AAA-6189-4F1A-ADBE-92E53ED2C510}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749E1764-BA27-EF40-A5DB-01845CB07B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener" sheetId="2" r:id="rId1"/>
@@ -31,6 +31,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1468,42 +1478,42 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>49.5</v>
+            <v>52.93</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>542.659087</v>
+            <v>1269.4252260000001</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>26861.6248065</v>
+            <v>67190.677212180002</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-4235</v>
+            <v>4028.7079999999996</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>31096.6248065</v>
+            <v>63161.969212180004</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>San Jose, CA</v>
+            <v>Ottowa, Canada</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>1995</v>
+            <v>2004</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>1998</v>
+            <v>2015</v>
           </cell>
         </row>
         <row r="28">
@@ -1511,78 +1521,74 @@
             <v>Q322</v>
           </cell>
           <cell r="D28">
-            <v>37561</v>
+            <v>46661</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>5.5350555958170204</v>
+            <v>7.729278198315245</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>2.7138436862497475</v>
+            <v>12.810644455706582</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>3.1417079012426754</v>
+            <v>12.042526794965024</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>-421.2402023888468</v>
+            <v>-3.3644129896469788</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1110.5937430892857</v>
+            <v>-19.688678338041829</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="20">
-          <cell r="AC20">
-            <v>1725</v>
-          </cell>
-          <cell r="AD20">
-            <v>7266</v>
-          </cell>
-          <cell r="AE20">
-            <v>-1347</v>
-          </cell>
-        </row>
-        <row r="25">
-          <cell r="AW25">
-            <v>0.08</v>
-          </cell>
-        </row>
-        <row r="27">
-          <cell r="U27">
-            <v>0.72890843662534988</v>
+          <cell r="AB20">
+            <v>2914.6589999999997</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="AP24">
+            <v>7.0000000000000007E-2</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="U28">
-            <v>0.2646941223510596</v>
+          <cell r="AP28">
+            <v>26.075206575494708</v>
           </cell>
         </row>
         <row r="29">
           <cell r="U29">
-            <v>0.10555777688924431</v>
-          </cell>
-          <cell r="AW29">
-            <v>57.281112716189718</v>
+            <v>0.48479871175523354</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="U30">
-            <v>0.34792626728110598</v>
-          </cell>
-        </row>
-        <row r="31">
-          <cell r="AW31">
-            <v>0.15719419628666098</v>
+          <cell r="AP30">
+            <v>-0.50736431937474569</v>
+          </cell>
+        </row>
+        <row r="32">
+          <cell r="U32">
+            <v>-0.2527931488801054</v>
+          </cell>
+        </row>
+        <row r="33">
+          <cell r="U33">
+            <v>-0.11594861660079051</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="U34">
+            <v>-8.1205093774064027E-3</v>
           </cell>
         </row>
       </sheetData>
@@ -1602,42 +1608,42 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>52.93</v>
+            <v>49.5</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>1269.4252260000001</v>
+            <v>542.659087</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>67190.677212180002</v>
+            <v>26861.6248065</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>4028.7079999999996</v>
+            <v>-4235</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>63161.969212180004</v>
+            <v>31096.6248065</v>
           </cell>
         </row>
         <row r="23">
           <cell r="C23" t="str">
-            <v>Ottowa, Canada</v>
+            <v>San Jose, CA</v>
           </cell>
         </row>
         <row r="24">
           <cell r="C24">
-            <v>2004</v>
+            <v>1995</v>
           </cell>
         </row>
         <row r="25">
           <cell r="C25">
-            <v>2015</v>
+            <v>1998</v>
           </cell>
         </row>
         <row r="28">
@@ -1645,19 +1651,78 @@
             <v>Q322</v>
           </cell>
           <cell r="D28">
-            <v>46661</v>
+            <v>37561</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>7.729278198315245</v>
+            <v>5.5350555958170204</v>
+          </cell>
+        </row>
+        <row r="34">
+          <cell r="C34">
+            <v>2.7138436862497475</v>
+          </cell>
+        </row>
+        <row r="35">
+          <cell r="C35">
+            <v>3.1417079012426754</v>
+          </cell>
+        </row>
+        <row r="36">
+          <cell r="C36">
+            <v>-421.2402023888468</v>
+          </cell>
+        </row>
+        <row r="37">
+          <cell r="C37">
+            <v>1110.5937430892857</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="20">
+          <cell r="AC20">
+            <v>1725</v>
+          </cell>
+          <cell r="AD20">
+            <v>7266</v>
+          </cell>
+          <cell r="AE20">
+            <v>-1347</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="AW25">
+            <v>0.08</v>
+          </cell>
+        </row>
+        <row r="27">
+          <cell r="U27">
+            <v>0.72890843662534988</v>
+          </cell>
+        </row>
+        <row r="28">
+          <cell r="U28">
+            <v>0.2646941223510596</v>
+          </cell>
+        </row>
         <row r="29">
           <cell r="U29">
-            <v>0.48479871175523354</v>
+            <v>0.10555777688924431</v>
+          </cell>
+          <cell r="AW29">
+            <v>57.281112716189718</v>
+          </cell>
+        </row>
+        <row r="30">
+          <cell r="U30">
+            <v>0.34792626728110598</v>
+          </cell>
+        </row>
+        <row r="31">
+          <cell r="AW31">
+            <v>0.15719419628666098</v>
           </cell>
         </row>
       </sheetData>
@@ -1972,9 +2037,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1986,39 +2051,39 @@
   <dimension ref="A1:AM55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AC22" sqref="AC22"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.140625" style="1"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="27" customWidth="1"/>
-    <col min="14" max="15" width="9.42578125" style="28" customWidth="1"/>
-    <col min="16" max="23" width="9.42578125" style="5" customWidth="1"/>
-    <col min="24" max="27" width="9.42578125" style="23" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="1"/>
-    <col min="29" max="32" width="9.140625" style="5"/>
-    <col min="33" max="33" width="9.140625" style="1"/>
-    <col min="34" max="35" width="9.140625" style="5"/>
-    <col min="36" max="36" width="19.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="1"/>
-    <col min="38" max="38" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.1640625" style="5"/>
+    <col min="6" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.1640625" style="1"/>
+    <col min="11" max="11" width="9.1640625" style="5"/>
+    <col min="12" max="12" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="27" customWidth="1"/>
+    <col min="14" max="15" width="9.5" style="28" customWidth="1"/>
+    <col min="16" max="23" width="9.5" style="5" customWidth="1"/>
+    <col min="24" max="27" width="9.5" style="23" customWidth="1"/>
+    <col min="28" max="28" width="9.1640625" style="1"/>
+    <col min="29" max="32" width="9.1640625" style="5"/>
+    <col min="33" max="33" width="9.1640625" style="1"/>
+    <col min="34" max="35" width="9.1640625" style="5"/>
+    <col min="36" max="36" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="9.1640625" style="1"/>
+    <col min="38" max="38" width="16.5" style="5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="1"/>
+    <col min="40" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="F1" s="35" t="s">
         <v>29</v>
       </c>
@@ -2035,7 +2100,7 @@
       <c r="AA1" s="35"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2140,7 +2205,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
       <c r="F3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -2151,7 +2216,7 @@
       <c r="AA3" s="24"/>
       <c r="AM3" s="5"/>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
@@ -2166,7 +2231,7 @@
       </c>
       <c r="F4" s="16">
         <f>[1]Main!$C$6*F54</f>
-        <v>155.31750000000002</v>
+        <v>159.1525</v>
       </c>
       <c r="G4" s="19">
         <f>[1]Main!$C$7</f>
@@ -2174,15 +2239,15 @@
       </c>
       <c r="H4" s="17">
         <f>[1]Main!$C$8*F54</f>
-        <v>10703.987103127502</v>
+        <v>10968.283080982501</v>
       </c>
       <c r="I4" s="17">
         <f>[1]Main!$C$11*F54</f>
-        <v>525.27690000000007</v>
+        <v>538.24670000000003</v>
       </c>
       <c r="J4" s="17">
         <f>[1]Main!$C$12*F54</f>
-        <v>10178.710203127501</v>
+        <v>10430.036380982501</v>
       </c>
       <c r="K4" s="5" t="str">
         <f>[1]Main!$C$28</f>
@@ -2194,7 +2259,7 @@
       </c>
       <c r="M4" s="27">
         <f>'[1]Financial Model'!$AU$27*F54</f>
-        <v>144.21036736217536</v>
+        <v>147.7711171735871</v>
       </c>
       <c r="N4" s="32">
         <f>'[1]Financial Model'!$AU$29</f>
@@ -2220,11 +2285,11 @@
       <c r="W4" s="22"/>
       <c r="X4" s="24">
         <f>'[1]Financial Model'!$AH$21*F54</f>
-        <v>-248.56146000000001</v>
+        <v>-254.69877999999997</v>
       </c>
       <c r="Y4" s="24">
         <f>'[1]Financial Model'!$AG$15*F54</f>
-        <v>-169.53623999999999</v>
+        <v>-173.72231999999997</v>
       </c>
       <c r="Z4" s="24"/>
       <c r="AA4" s="24"/>
@@ -2263,7 +2328,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
         <v>80</v>
       </c>
@@ -2278,7 +2343,7 @@
       </c>
       <c r="F5" s="16">
         <f>[2]Main!$C$6*F54</f>
-        <v>3.2561999999999998</v>
+        <v>3.3365999999999993</v>
       </c>
       <c r="G5" s="17">
         <f>[2]Main!$C$7</f>
@@ -2286,15 +2351,15 @@
       </c>
       <c r="H5" s="17">
         <f>[2]Main!$C$8*F54</f>
-        <v>191.46897866340001</v>
+        <v>196.19660776619997</v>
       </c>
       <c r="I5" s="17">
         <f>[2]Main!$C$11*F54</f>
-        <v>12.968910000000001</v>
+        <v>13.289129999999998</v>
       </c>
       <c r="J5" s="17">
         <f>[2]Main!$C$12*F54</f>
-        <v>178.50006866340001</v>
+        <v>182.90747776619997</v>
       </c>
       <c r="K5" s="5" t="str">
         <f>[2]Main!$C$28</f>
@@ -2356,7 +2421,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
       <c r="F6" s="16"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -2371,7 +2436,7 @@
       <c r="AA6" s="24"/>
       <c r="AM6" s="5"/>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2386,7 +2451,7 @@
       </c>
       <c r="F7" s="16">
         <f>[3]Main!$C$6*$F$54</f>
-        <v>48.114000000000004</v>
+        <v>49.302</v>
       </c>
       <c r="G7" s="17">
         <f>[3]Main!$C$7</f>
@@ -2394,15 +2459,15 @@
       </c>
       <c r="H7" s="17">
         <f>[3]Main!$C$8*$F$54</f>
-        <v>8838.1840242960006</v>
+        <v>9056.4107903280001</v>
       </c>
       <c r="I7" s="17">
         <f>[3]Main!$C$11*F54</f>
-        <v>2589.3415800000002</v>
+        <v>2653.2759399999995</v>
       </c>
       <c r="J7" s="17">
         <f>[3]Main!$C$12*F54</f>
-        <v>6248.8424442960013</v>
+        <v>6403.1348503280005</v>
       </c>
       <c r="K7" s="5" t="str">
         <f>[3]Main!$C$28</f>
@@ -2414,7 +2479,7 @@
       </c>
       <c r="M7" s="27">
         <f>'[3]Financial Model'!$AP$29*F54</f>
-        <v>42.985358058347664</v>
+        <v>44.04672492398587</v>
       </c>
       <c r="N7" s="32">
         <f>'[3]Financial Model'!$AP$31</f>
@@ -2449,19 +2514,19 @@
       <c r="W7" s="22"/>
       <c r="X7" s="24">
         <f>'[3]Financial Model'!$AB$17*$F$54</f>
-        <v>-769.4190000000001</v>
+        <v>-788.41700000000003</v>
       </c>
       <c r="Y7" s="24">
         <f>'[3]Financial Model'!$AA$17*$F$54</f>
-        <v>-397.6929899999999</v>
+        <v>-407.51256999999981</v>
       </c>
       <c r="Z7" s="24">
         <f>'[3]Financial Model'!$Z$17*$F$54</f>
-        <v>-248.72102999999996</v>
+        <v>-254.86228999999994</v>
       </c>
       <c r="AA7" s="24">
         <f>'[3]Financial Model'!$Y$17*F54</f>
-        <v>-98.778690000000012</v>
+        <v>-101.21767</v>
       </c>
       <c r="AC7" s="18">
         <f>'[3]Financial Model'!$U$24</f>
@@ -2498,7 +2563,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B8" s="7"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
@@ -2526,7 +2591,7 @@
       <c r="AF8" s="18"/>
       <c r="AM8" s="5"/>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2552,7 +2617,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2574,7 +2639,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -2704,12 +2769,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B12" s="7"/>
       <c r="F12" s="16"/>
       <c r="AM12" s="5"/>
     </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
@@ -2739,7 +2804,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -2759,7 +2824,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:39" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2779,7 +2844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
@@ -2794,7 +2859,7 @@
       </c>
       <c r="F19" s="17">
         <f>[5]Main!$C$6*F54</f>
-        <v>30.140100000000004</v>
+        <v>30.8843</v>
       </c>
       <c r="G19" s="17">
         <f>[5]Main!$C$7</f>
@@ -2802,15 +2867,15 @@
       </c>
       <c r="H19" s="17">
         <f>[5]Main!$C$8*F54</f>
-        <v>18017.118837900001</v>
+        <v>18461.985969699999</v>
       </c>
       <c r="I19" s="17">
         <f>[5]Main!$C$11*F54</f>
-        <v>1646.60364</v>
+        <v>1687.26052</v>
       </c>
       <c r="J19" s="17">
         <f>[5]Main!$C$12*F54</f>
-        <v>16370.5151979</v>
+        <v>16774.725449699999</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>[5]Main!$G$11</f>
@@ -2822,7 +2887,7 @@
       </c>
       <c r="M19" s="27">
         <f>'[5]Financial Model'!$AP$26*F54</f>
-        <v>53.598836857595423</v>
+        <v>54.922264928153325</v>
       </c>
       <c r="N19" s="32">
         <f>'[5]Financial Model'!$AP$28</f>
@@ -2842,11 +2907,11 @@
       </c>
       <c r="X19" s="25">
         <f>'[5]Financial Model'!$W$18*F54</f>
-        <v>-407.82689999999997</v>
+        <v>-417.89669999999995</v>
       </c>
       <c r="Y19" s="25">
         <f>'[5]Financial Model'!$V$18*F54</f>
-        <v>-211.26095999999995</v>
+        <v>-216.47727999999992</v>
       </c>
       <c r="Z19" s="23" t="s">
         <v>139</v>
@@ -2889,7 +2954,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2904,7 +2969,7 @@
       </c>
       <c r="F20" s="17">
         <f>[6]Main!$C$6*F54</f>
-        <v>27.078300000000002</v>
+        <v>27.7469</v>
       </c>
       <c r="G20" s="17">
         <f>[6]Main!$C$7</f>
@@ -2912,15 +2977,15 @@
       </c>
       <c r="H20" s="17">
         <f>[6]Main!$C$8*F54</f>
-        <v>8015.5288991349007</v>
+        <v>8213.4431929407001</v>
       </c>
       <c r="I20" s="19">
         <f>[6]Main!$C$11*F54</f>
-        <v>-425.90609999999998</v>
+        <v>-436.42229999999995</v>
       </c>
       <c r="J20" s="17">
         <f>[6]Main!$C$12*F54</f>
-        <v>8441.4349991349009</v>
+        <v>8649.8654929407003</v>
       </c>
       <c r="K20" s="26" t="str">
         <f>[6]Main!$C$26</f>
@@ -2937,7 +3002,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
@@ -2951,178 +3016,222 @@
         <v>17</v>
       </c>
       <c r="F22" s="16">
-        <f>[8]Main!$C$6*$F$54</f>
-        <v>42.8733</v>
+        <f>[7]Main!$C$6*$F$54</f>
+        <v>43.931899999999999</v>
       </c>
       <c r="G22" s="17">
+        <f>[7]Main!$C$7</f>
+        <v>1269.4252260000001</v>
+      </c>
+      <c r="H22" s="17">
+        <f>[7]Main!$C$8*F54</f>
+        <v>55768.262086109396</v>
+      </c>
+      <c r="I22" s="17">
+        <f>[7]Main!$C$11*F54</f>
+        <v>3343.8276399999995</v>
+      </c>
+      <c r="J22" s="17">
+        <f>[7]Main!$C$12*F54</f>
+        <v>52424.434446109401</v>
+      </c>
+      <c r="K22" s="5" t="str">
+        <f>[7]Main!$C$28</f>
+        <v>Q322</v>
+      </c>
+      <c r="L22" s="8">
+        <f>[7]Main!$D$28</f>
+        <v>46661</v>
+      </c>
+      <c r="M22" s="27">
+        <f>'[7]Financial Model'!$AP$28</f>
+        <v>26.075206575494708</v>
+      </c>
+      <c r="N22" s="32">
+        <f>'[7]Financial Model'!$AP$30</f>
+        <v>-0.50736431937474569</v>
+      </c>
+      <c r="O22" s="32">
+        <f>'[7]Financial Model'!$AP$24</f>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="Q22" s="21">
+        <f>[7]Main!$C$33</f>
+        <v>7.729278198315245</v>
+      </c>
+      <c r="R22" s="21">
+        <f>[7]Main!$C$34</f>
+        <v>12.810644455706582</v>
+      </c>
+      <c r="S22" s="21">
+        <f>[7]Main!$C$35</f>
+        <v>12.042526794965024</v>
+      </c>
+      <c r="T22" s="21">
+        <f>[7]Main!$C$36</f>
+        <v>-3.3644129896469788</v>
+      </c>
+      <c r="U22" s="21">
+        <f>[7]Main!$C$37</f>
+        <v>-19.688678338041829</v>
+      </c>
+      <c r="X22" s="25">
+        <f>'[7]Financial Model'!$AB$20*F54</f>
+        <v>2419.1669699999998</v>
+      </c>
+      <c r="AC22" s="18">
+        <f>'[7]Financial Model'!$U$29</f>
+        <v>0.48479871175523354</v>
+      </c>
+      <c r="AD22" s="18">
+        <f>'[7]Financial Model'!$U$32</f>
+        <v>-0.2527931488801054</v>
+      </c>
+      <c r="AE22" s="18">
+        <f>'[7]Financial Model'!$U$33</f>
+        <v>-0.11594861660079051</v>
+      </c>
+      <c r="AF22" s="18">
+        <f>'[7]Financial Model'!$U$34</f>
+        <v>-8.1205093774064027E-3</v>
+      </c>
+      <c r="AH22" s="5">
+        <f>[7]Main!$C$24</f>
+        <v>2004</v>
+      </c>
+      <c r="AI22" s="5">
+        <f>[7]Main!$C$25</f>
+        <v>2015</v>
+      </c>
+      <c r="AJ22" s="5" t="str">
+        <f>[7]Main!$C$23</f>
+        <v>Ottowa, Canada</v>
+      </c>
+      <c r="AL22" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AM22" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="B23" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="16">
+        <f>[8]Main!$C$6*F54</f>
+        <v>41.085000000000001</v>
+      </c>
+      <c r="G23" s="19">
         <f>[8]Main!$C$7</f>
-        <v>1269.4252260000001</v>
-      </c>
-      <c r="H22" s="17">
+        <v>542.659087</v>
+      </c>
+      <c r="H23" s="17">
         <f>[8]Main!$C$8*F54</f>
-        <v>54424.448541865808</v>
-      </c>
-      <c r="I22" s="17">
+        <v>22295.148589394998</v>
+      </c>
+      <c r="I23" s="17">
         <f>[8]Main!$C$11*F54</f>
-        <v>3263.2534799999999</v>
-      </c>
-      <c r="J22" s="17">
+        <v>-3515.0499999999997</v>
+      </c>
+      <c r="J23" s="17">
         <f>[8]Main!$C$12*F54</f>
-        <v>51161.195061865808</v>
-      </c>
-      <c r="K22" s="5" t="str">
+        <v>25810.198589395</v>
+      </c>
+      <c r="K23" s="5" t="str">
         <f>[8]Main!$C$28</f>
         <v>Q322</v>
       </c>
-      <c r="L22" s="8">
+      <c r="L23" s="8">
         <f>[8]Main!$D$28</f>
-        <v>46661</v>
-      </c>
-      <c r="Q22" s="21">
-        <f>[8]Main!$C$33</f>
-        <v>7.729278198315245</v>
-      </c>
-      <c r="AC22" s="18">
-        <f>'[8]Financial Model'!$U$29</f>
-        <v>0.48479871175523354</v>
-      </c>
-      <c r="AH22" s="5">
-        <f>[8]Main!$C$24</f>
-        <v>2004</v>
-      </c>
-      <c r="AI22" s="5">
-        <f>[8]Main!$C$25</f>
-        <v>2015</v>
-      </c>
-      <c r="AJ22" s="5" t="str">
-        <f>[8]Main!$C$23</f>
-        <v>Ottowa, Canada</v>
-      </c>
-      <c r="AL22" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="AM22" s="5" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.2">
-      <c r="B23" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="16">
-        <f>[7]Main!$C$6*F54</f>
-        <v>40.095000000000006</v>
-      </c>
-      <c r="G23" s="19">
-        <f>[7]Main!$C$7</f>
-        <v>542.659087</v>
-      </c>
-      <c r="H23" s="17">
-        <f>[7]Main!$C$8*F54</f>
-        <v>21757.916093265001</v>
-      </c>
-      <c r="I23" s="17">
-        <f>[7]Main!$C$11*F54</f>
-        <v>-3430.3500000000004</v>
-      </c>
-      <c r="J23" s="17">
-        <f>[7]Main!$C$12*F54</f>
-        <v>25188.266093265003</v>
-      </c>
-      <c r="K23" s="5" t="str">
-        <f>[7]Main!$C$28</f>
-        <v>Q322</v>
-      </c>
-      <c r="L23" s="8">
-        <f>[7]Main!$D$28</f>
         <v>37561</v>
       </c>
       <c r="M23" s="27">
-        <f>'[7]Financial Model'!$AW$29*$F$54</f>
-        <v>46.397701300113674</v>
+        <f>'[8]Financial Model'!$AW$29*$F$54</f>
+        <v>47.543323554437464</v>
       </c>
       <c r="N23" s="32">
-        <f>'[7]Financial Model'!$AW$31</f>
+        <f>'[8]Financial Model'!$AW$31</f>
         <v>0.15719419628666098</v>
       </c>
       <c r="O23" s="32">
-        <f>'[7]Financial Model'!$AW$25</f>
+        <f>'[8]Financial Model'!$AW$25</f>
         <v>0.08</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="21">
-        <f>[7]Main!$C$33</f>
+        <f>[8]Main!$C$33</f>
         <v>5.5350555958170204</v>
       </c>
       <c r="R23" s="21">
-        <f>[7]Main!$C$34</f>
+        <f>[8]Main!$C$34</f>
         <v>2.7138436862497475</v>
       </c>
       <c r="S23" s="21">
-        <f>[7]Main!$C$35</f>
+        <f>[8]Main!$C$35</f>
         <v>3.1417079012426754</v>
       </c>
       <c r="T23" s="21">
-        <f>[7]Main!$C$36</f>
+        <f>[8]Main!$C$36</f>
         <v>-421.2402023888468</v>
       </c>
       <c r="U23" s="21">
-        <f>[7]Main!$C$37</f>
+        <f>[8]Main!$C$37</f>
         <v>1110.5937430892857</v>
       </c>
       <c r="V23" s="8"/>
       <c r="W23" s="8"/>
       <c r="X23" s="25">
-        <f>'[7]Financial Model'!$AE$20*F54</f>
-        <v>-1091.0700000000002</v>
+        <f>'[8]Financial Model'!$AE$20*F54</f>
+        <v>-1118.01</v>
       </c>
       <c r="Y23" s="25">
-        <f>'[7]Financial Model'!$AD$20*F54</f>
-        <v>5885.46</v>
+        <f>'[8]Financial Model'!$AD$20*F54</f>
+        <v>6030.78</v>
       </c>
       <c r="Z23" s="25">
-        <f>'[7]Financial Model'!$AC$20*F54</f>
-        <v>1397.25</v>
+        <f>'[8]Financial Model'!$AC$20*F54</f>
+        <v>1431.75</v>
       </c>
       <c r="AA23" s="25">
-        <f>'[7]Financial Model'!$AC$20*G54</f>
-        <v>2129.6296296296296</v>
+        <f>'[8]Financial Model'!$AC$20*G54</f>
+        <v>2078.3132530120483</v>
       </c>
       <c r="AC23" s="18">
-        <f>'[7]Financial Model'!$U$27</f>
+        <f>'[8]Financial Model'!$U$27</f>
         <v>0.72890843662534988</v>
       </c>
       <c r="AD23" s="18">
-        <f>'[7]Financial Model'!$U$28</f>
+        <f>'[8]Financial Model'!$U$28</f>
         <v>0.2646941223510596</v>
       </c>
       <c r="AE23" s="18">
-        <f>'[7]Financial Model'!$U$29</f>
+        <f>'[8]Financial Model'!$U$29</f>
         <v>0.10555777688924431</v>
       </c>
       <c r="AF23" s="18">
-        <f>'[7]Financial Model'!$U$30</f>
+        <f>'[8]Financial Model'!$U$30</f>
         <v>0.34792626728110598</v>
       </c>
       <c r="AH23" s="5">
-        <f>[7]Main!$C$24</f>
+        <f>[8]Main!$C$24</f>
         <v>1995</v>
       </c>
       <c r="AI23" s="5">
-        <f>[7]Main!$C$25</f>
+        <f>[8]Main!$C$25</f>
         <v>1998</v>
       </c>
       <c r="AJ23" s="5" t="str">
-        <f>[7]Main!$C$23</f>
+        <f>[8]Main!$C$23</f>
         <v>San Jose, CA</v>
       </c>
       <c r="AL23" s="5" t="s">
@@ -3132,7 +3241,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -3152,7 +3261,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
@@ -3170,7 +3279,7 @@
       </c>
       <c r="AM25" s="5"/>
     </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
@@ -3185,7 +3294,7 @@
       </c>
       <c r="AM26" s="5"/>
     </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
@@ -3197,7 +3306,7 @@
       </c>
       <c r="AM27" s="5"/>
     </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -3214,7 +3323,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3231,7 +3340,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>106</v>
       </c>
@@ -3248,7 +3357,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>108</v>
       </c>
@@ -3271,7 +3380,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>110</v>
       </c>
@@ -3288,7 +3397,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3327,17 +3436,17 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G40" s="19"/>
       <c r="H40" s="17"/>
       <c r="AM40" s="5"/>
     </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G41" s="19"/>
       <c r="H41" s="17"/>
       <c r="AM41" s="5"/>
     </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>121</v>
       </c>
@@ -3352,14 +3461,14 @@
       </c>
       <c r="F42" s="16">
         <f>332.82*F54</f>
-        <v>269.58420000000001</v>
+        <v>276.24059999999997</v>
       </c>
       <c r="G42" s="19">
         <v>445.02</v>
       </c>
       <c r="H42" s="17">
         <f>G42*F42</f>
-        <v>119970.360684</v>
+        <v>122932.59181199998</v>
       </c>
       <c r="AL42" s="5" t="s">
         <v>126</v>
@@ -3368,7 +3477,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
@@ -3383,14 +3492,14 @@
       </c>
       <c r="F43" s="16">
         <f>92.06*F54</f>
-        <v>74.568600000000004</v>
+        <v>76.409800000000004</v>
       </c>
       <c r="G43" s="19">
         <v>193.13</v>
       </c>
       <c r="H43" s="17">
         <f>G43*F43</f>
-        <v>14401.433718</v>
+        <v>14757.024674</v>
       </c>
       <c r="AL43" s="5" t="s">
         <v>126</v>
@@ -3399,7 +3508,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
@@ -3429,12 +3538,12 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:39" x14ac:dyDescent="0.15">
       <c r="G45" s="19"/>
       <c r="H45" s="17"/>
       <c r="AM45" s="5"/>
     </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
@@ -3445,7 +3554,7 @@
       <c r="H46" s="17"/>
       <c r="AM46" s="5"/>
     </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
@@ -3456,7 +3565,7 @@
       <c r="H47" s="17"/>
       <c r="AM47" s="5"/>
     </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:39" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
@@ -3467,12 +3576,12 @@
       <c r="H48" s="17"/>
       <c r="AM48" s="5"/>
     </row>
-    <row r="49" spans="5:39" x14ac:dyDescent="0.2">
+    <row r="49" spans="5:39" x14ac:dyDescent="0.15">
       <c r="G49" s="19"/>
       <c r="H49" s="17"/>
       <c r="AM49" s="5"/>
     </row>
-    <row r="53" spans="5:39" x14ac:dyDescent="0.2">
+    <row r="53" spans="5:39" x14ac:dyDescent="0.15">
       <c r="E53" s="33" t="s">
         <v>25</v>
       </c>
@@ -3481,19 +3590,19 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="5:39" x14ac:dyDescent="0.2">
+    <row r="54" spans="5:39" x14ac:dyDescent="0.15">
       <c r="E54" s="10" t="s">
         <v>27</v>
       </c>
       <c r="F54" s="11">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="G54" s="12">
         <f>1/F54</f>
-        <v>1.2345679012345678</v>
-      </c>
-    </row>
-    <row r="55" spans="5:39" x14ac:dyDescent="0.2">
+        <v>1.2048192771084338</v>
+      </c>
+    </row>
+    <row r="55" spans="5:39" x14ac:dyDescent="0.15">
       <c r="E55" s="13" t="s">
         <v>28</v>
       </c>
@@ -3537,21 +3646,21 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.140625" style="1"/>
+    <col min="4" max="8" width="9.1640625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3584,7 +3693,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -3610,11 +3719,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Add revenue growth columns
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{749E1764-BA27-EF40-A5DB-01845CB07B57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F2D308-9237-4CD9-9DFA-78CB279C6423}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener" sheetId="2" r:id="rId1"/>
@@ -32,22 +32,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="150">
   <si>
     <t>Ticker</t>
   </si>
@@ -479,6 +469,24 @@
   </si>
   <si>
     <t>Discount</t>
+  </si>
+  <si>
+    <t>RevG [C]</t>
+  </si>
+  <si>
+    <t>RevG 22</t>
+  </si>
+  <si>
+    <t>RevG21</t>
+  </si>
+  <si>
+    <t>RevG 20</t>
+  </si>
+  <si>
+    <t>RevG 19</t>
+  </si>
+  <si>
+    <t>RevG18</t>
   </si>
 </sst>
 </file>
@@ -716,7 +724,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -807,6 +815,9 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -909,6 +920,14 @@
             <v>0.08</v>
           </cell>
         </row>
+        <row r="26">
+          <cell r="Y26">
+            <v>0.47038912615197459</v>
+          </cell>
+          <cell r="AH26">
+            <v>0.48003319895660423</v>
+          </cell>
+        </row>
         <row r="27">
           <cell r="AU27">
             <v>178.03749057058687</v>
@@ -1007,6 +1026,11 @@
         </row>
       </sheetData>
       <sheetData sheetId="1">
+        <row r="25">
+          <cell r="J25">
+            <v>0.21252241299870667</v>
+          </cell>
+        </row>
         <row r="28">
           <cell r="J28">
             <v>0.68957308000457829</v>
@@ -1132,6 +1156,20 @@
             <v>-949.90000000000009</v>
           </cell>
         </row>
+        <row r="21">
+          <cell r="U21">
+            <v>0.32810304576208882</v>
+          </cell>
+          <cell r="Z21">
+            <v>0.74515549935622039</v>
+          </cell>
+          <cell r="AA21">
+            <v>0.55295345483521796</v>
+          </cell>
+          <cell r="AB21">
+            <v>0.613053532344634</v>
+          </cell>
+        </row>
         <row r="24">
           <cell r="U24">
             <v>0.47005177868427206</v>
@@ -1166,7 +1204,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
+      <sheetData sheetId="2" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1297,6 +1335,21 @@
           </cell>
         </row>
         <row r="22">
+          <cell r="J22">
+            <v>0.11441144114411439</v>
+          </cell>
+          <cell r="S22">
+            <v>4.8754062838569867E-2</v>
+          </cell>
+          <cell r="T22">
+            <v>-1.7045454545454586E-2</v>
+          </cell>
+          <cell r="U22">
+            <v>-2.9952706253284278E-2</v>
+          </cell>
+          <cell r="V22">
+            <v>5.4712892741061836E-2</v>
+          </cell>
           <cell r="AH22">
             <v>6.3308923646501336</v>
           </cell>
@@ -1353,7 +1406,6 @@
           <cell r="G11" t="str">
             <v>Q322</v>
           </cell>
-          <cell r="H11"/>
         </row>
         <row r="12">
           <cell r="C12">
@@ -1409,6 +1461,12 @@
           </cell>
         </row>
         <row r="28">
+          <cell r="M28">
+            <v>1.6435123376317362E-2</v>
+          </cell>
+          <cell r="W28">
+            <v>1.0772942519902369</v>
+          </cell>
           <cell r="AP28">
             <v>0.77832312625357636</v>
           </cell>
@@ -1557,6 +1615,12 @@
           </cell>
         </row>
         <row r="24">
+          <cell r="U24">
+            <v>0.2157616530514177</v>
+          </cell>
+          <cell r="AB24">
+            <v>0.57428577182862139</v>
+          </cell>
           <cell r="AP24">
             <v>7.0000000000000007E-2</v>
           </cell>
@@ -1690,6 +1754,23 @@
           </cell>
           <cell r="AE20">
             <v>-1347</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="Y24">
+            <v>-4.8380647740903671E-2</v>
+          </cell>
+          <cell r="AF24">
+            <v>8.2502266545784186E-2</v>
+          </cell>
+          <cell r="AG24">
+            <v>-0.14805509026614549</v>
+          </cell>
+          <cell r="AH24">
+            <v>0.17018022938285093</v>
+          </cell>
+          <cell r="AI24">
+            <v>-2.7349948660505885E-2</v>
           </cell>
         </row>
         <row r="25">
@@ -2037,9 +2118,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2048,42 +2129,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1873CD5B-C727-4CC0-ACC4-210B76523995}">
-  <dimension ref="A1:AM55"/>
+  <dimension ref="A1:AT55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="AJ20" sqref="AJ20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="5"/>
-    <col min="6" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="9.1640625" style="1"/>
-    <col min="11" max="11" width="9.1640625" style="5"/>
-    <col min="12" max="12" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="27" customWidth="1"/>
-    <col min="14" max="15" width="9.5" style="28" customWidth="1"/>
-    <col min="16" max="23" width="9.5" style="5" customWidth="1"/>
-    <col min="24" max="27" width="9.5" style="23" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" style="1"/>
-    <col min="29" max="32" width="9.1640625" style="5"/>
-    <col min="33" max="33" width="9.1640625" style="1"/>
-    <col min="34" max="35" width="9.1640625" style="5"/>
-    <col min="36" max="36" width="19.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.1640625" style="1"/>
-    <col min="38" max="38" width="16.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="5" width="9.140625" style="5"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="27" customWidth="1"/>
+    <col min="14" max="15" width="9.42578125" style="28" customWidth="1"/>
+    <col min="16" max="23" width="9.42578125" style="5" customWidth="1"/>
+    <col min="24" max="27" width="9.42578125" style="23" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1"/>
+    <col min="29" max="32" width="9.140625" style="5"/>
+    <col min="33" max="33" width="9.140625" style="1"/>
+    <col min="34" max="39" width="9.140625" style="18"/>
+    <col min="40" max="40" width="9.140625" style="1"/>
+    <col min="41" max="42" width="9.140625" style="5"/>
+    <col min="43" max="43" width="21" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="1"/>
+    <col min="45" max="45" width="16.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F1" s="35" t="s">
         <v>29</v>
       </c>
@@ -2100,7 +2183,7 @@
       <c r="AA1" s="35"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:39" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2189,23 +2272,41 @@
       <c r="AF2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AH2" s="36" t="s">
+        <v>144</v>
+      </c>
+      <c r="AI2" s="36" t="s">
+        <v>145</v>
+      </c>
+      <c r="AJ2" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="AK2" s="36" t="s">
+        <v>147</v>
+      </c>
+      <c r="AL2" s="36" t="s">
+        <v>148</v>
+      </c>
+      <c r="AM2" s="36" t="s">
+        <v>149</v>
+      </c>
+      <c r="AO2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AJ2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="F3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -2214,9 +2315,9 @@
       <c r="Y3" s="24"/>
       <c r="Z3" s="24"/>
       <c r="AA3" s="24"/>
-      <c r="AM3" s="5"/>
-    </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AT3" s="5"/>
+    </row>
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
@@ -2309,26 +2410,34 @@
         <f>'[1]Financial Model'!$X$32</f>
         <v>-2.6326241624645998E-2</v>
       </c>
-      <c r="AH4" s="5">
+      <c r="AH4" s="18">
+        <f>'[1]Financial Model'!$Y$26</f>
+        <v>0.47038912615197459</v>
+      </c>
+      <c r="AJ4" s="18">
+        <f>'[1]Financial Model'!$AH$26</f>
+        <v>0.48003319895660423</v>
+      </c>
+      <c r="AO4" s="5">
         <f>[1]Main!$C24</f>
         <v>2007</v>
       </c>
-      <c r="AI4" s="5">
+      <c r="AP4" s="5">
         <f>[1]Main!$C$25</f>
         <v>2017</v>
       </c>
-      <c r="AJ4" s="5" t="str">
+      <c r="AQ4" s="5" t="str">
         <f>[1]Main!$C$23</f>
         <v>New York City, NY</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AS4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AM4" s="5" t="s">
+      <c r="AT4" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>80</v>
       </c>
@@ -2402,26 +2511,30 @@
         <f>'[2]Financial Model'!$J$31</f>
         <v>-1.6676961087090797E-3</v>
       </c>
-      <c r="AH5" s="5">
+      <c r="AH5" s="18">
+        <f>'[2]Financial Model'!$J$25</f>
+        <v>0.21252241299870667</v>
+      </c>
+      <c r="AO5" s="5">
         <f>[2]Main!$C$24</f>
         <v>2010</v>
       </c>
-      <c r="AI5" s="5">
+      <c r="AP5" s="5">
         <f>[2]Main!$C$25</f>
         <v>2022</v>
       </c>
-      <c r="AJ5" s="5" t="str">
+      <c r="AQ5" s="5" t="str">
         <f>[2]Main!$C$23</f>
         <v>Redwood City, CA</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AS5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AM5" s="5" t="s">
+      <c r="AT5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="F6" s="16"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -2434,9 +2547,9 @@
       <c r="Y6" s="24"/>
       <c r="Z6" s="24"/>
       <c r="AA6" s="24"/>
-      <c r="AM6" s="5"/>
-    </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AT6" s="5"/>
+    </row>
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2544,26 +2657,42 @@
         <f>'[3]Financial Model'!$U$27</f>
         <v>-7.4778536471246807E-3</v>
       </c>
-      <c r="AH7" s="5">
+      <c r="AH7" s="18">
+        <f>'[3]Financial Model'!$U$21</f>
+        <v>0.32810304576208882</v>
+      </c>
+      <c r="AJ7" s="18">
+        <f>'[3]Financial Model'!$AB$21</f>
+        <v>0.613053532344634</v>
+      </c>
+      <c r="AK7" s="18">
+        <f>'[3]Financial Model'!$AA$21</f>
+        <v>0.55295345483521796</v>
+      </c>
+      <c r="AL7" s="18">
+        <f>'[3]Financial Model'!$Z$21</f>
+        <v>0.74515549935622039</v>
+      </c>
+      <c r="AO7" s="5">
         <f>[3]Main!$C$24</f>
         <v>2008</v>
       </c>
-      <c r="AI7" s="5">
+      <c r="AP7" s="5">
         <f>[3]Main!$C$25</f>
         <v>2016</v>
       </c>
-      <c r="AJ7" s="5" t="str">
+      <c r="AQ7" s="5" t="str">
         <f>[3]Main!$C$23</f>
         <v>San Francisco, CA</v>
       </c>
-      <c r="AL7" s="5" t="s">
+      <c r="AS7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AM7" s="5" t="s">
+      <c r="AT7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
@@ -2589,9 +2718,9 @@
       <c r="AD8" s="18"/>
       <c r="AE8" s="18"/>
       <c r="AF8" s="18"/>
-      <c r="AM8" s="5"/>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AT8" s="5"/>
+    </row>
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2610,14 +2739,14 @@
       <c r="Y9" s="24"/>
       <c r="Z9" s="24"/>
       <c r="AA9" s="24"/>
-      <c r="AL9" s="5" t="s">
+      <c r="AS9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AM9" s="5" t="s">
+      <c r="AT9" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2632,14 +2761,14 @@
       <c r="Y10" s="24"/>
       <c r="Z10" s="24"/>
       <c r="AA10" s="24"/>
-      <c r="AL10" s="5" t="s">
+      <c r="AS10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AM10" s="5" t="s">
+      <c r="AT10" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -2750,31 +2879,51 @@
         <f>'[4]Financial Model'!$V$20</f>
         <v>0.24629080118694363</v>
       </c>
-      <c r="AH11" s="5">
+      <c r="AH11" s="18">
+        <f>'[4]Financial Model'!$J$22</f>
+        <v>0.11441144114411439</v>
+      </c>
+      <c r="AI11" s="18">
+        <f>'[4]Financial Model'!$V$22</f>
+        <v>5.4712892741061836E-2</v>
+      </c>
+      <c r="AJ11" s="18">
+        <f>'[4]Financial Model'!$U$22</f>
+        <v>-2.9952706253284278E-2</v>
+      </c>
+      <c r="AK11" s="18">
+        <f>'[4]Financial Model'!$T$22</f>
+        <v>-1.7045454545454586E-2</v>
+      </c>
+      <c r="AL11" s="18">
+        <f>'[4]Financial Model'!$S$22</f>
+        <v>4.8754062838569867E-2</v>
+      </c>
+      <c r="AO11" s="5">
         <f>[4]Main!$C$24</f>
         <v>1981</v>
       </c>
-      <c r="AI11" s="5">
+      <c r="AP11" s="5">
         <f>[4]Main!$C$25</f>
         <v>1989</v>
       </c>
-      <c r="AJ11" s="5" t="str">
+      <c r="AQ11" s="5" t="str">
         <f>[4]Main!$C$23</f>
         <v>Newcastle, UK</v>
       </c>
-      <c r="AL11" s="5" t="s">
+      <c r="AS11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AM11" s="5" t="s">
+      <c r="AT11" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="F12" s="16"/>
-      <c r="AM12" s="5"/>
-    </row>
-    <row r="13" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="AT12" s="5"/>
+    </row>
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
@@ -2787,24 +2936,24 @@
       <c r="E13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AH13" s="5">
+      <c r="AO13" s="5">
         <v>2002</v>
       </c>
-      <c r="AI13" s="5">
+      <c r="AP13" s="5">
         <v>2015</v>
       </c>
-      <c r="AJ13" s="5" t="str">
+      <c r="AQ13" s="5" t="str">
         <f>[3]Main!$C$23</f>
         <v>San Francisco, CA</v>
       </c>
-      <c r="AL13" s="5" t="s">
+      <c r="AS13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AM13" s="5" t="s">
+      <c r="AT13" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -2817,14 +2966,14 @@
       <c r="E15" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AL15" s="5" t="s">
+      <c r="AS15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AM15" s="5" t="s">
+      <c r="AT15" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:39" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
@@ -2837,14 +2986,14 @@
       <c r="E16" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AL16" s="5" t="s">
+      <c r="AS16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AM16" s="5" t="s">
+      <c r="AT16" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
@@ -2935,26 +3084,34 @@
         <f>'[5]Financial Model'!$M$25</f>
         <v>-1.1673022715967497E-3</v>
       </c>
-      <c r="AH19" s="5">
+      <c r="AH19" s="18">
+        <f>'[5]Financial Model'!$M$28</f>
+        <v>1.6435123376317362E-2</v>
+      </c>
+      <c r="AJ19" s="18">
+        <f>'[5]Financial Model'!$W$28</f>
+        <v>1.0772942519902369</v>
+      </c>
+      <c r="AO19" s="5">
         <f>[5]Main!$G$8</f>
         <v>2004</v>
       </c>
-      <c r="AI19" s="5">
+      <c r="AP19" s="5">
         <f>[5]Main!$G$7</f>
         <v>2021</v>
       </c>
-      <c r="AJ19" s="5" t="str">
+      <c r="AQ19" s="5" t="str">
         <f>[5]Main!$G$6</f>
         <v>San Mateo, CA</v>
       </c>
-      <c r="AL19" s="5" t="s">
+      <c r="AS19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AM19" s="5" t="s">
+      <c r="AT19" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
@@ -2995,14 +3152,14 @@
         <f>[6]Main!$D$26</f>
         <v>0</v>
       </c>
-      <c r="AL20" s="5" t="s">
+      <c r="AS20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AM20" s="5" t="s">
+      <c r="AT20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
@@ -3095,26 +3252,34 @@
         <f>'[7]Financial Model'!$U$34</f>
         <v>-8.1205093774064027E-3</v>
       </c>
-      <c r="AH22" s="5">
+      <c r="AH22" s="18">
+        <f>'[7]Financial Model'!$U$24</f>
+        <v>0.2157616530514177</v>
+      </c>
+      <c r="AJ22" s="18">
+        <f>'[7]Financial Model'!$AB$24</f>
+        <v>0.57428577182862139</v>
+      </c>
+      <c r="AO22" s="5">
         <f>[7]Main!$C$24</f>
         <v>2004</v>
       </c>
-      <c r="AI22" s="5">
+      <c r="AP22" s="5">
         <f>[7]Main!$C$25</f>
         <v>2015</v>
       </c>
-      <c r="AJ22" s="5" t="str">
+      <c r="AQ22" s="5" t="str">
         <f>[7]Main!$C$23</f>
         <v>Ottowa, Canada</v>
       </c>
-      <c r="AL22" s="5" t="s">
+      <c r="AS22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM22" s="5" t="s">
+      <c r="AT22" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>82</v>
       </c>
@@ -3222,26 +3387,46 @@
         <f>'[8]Financial Model'!$U$30</f>
         <v>0.34792626728110598</v>
       </c>
-      <c r="AH23" s="5">
+      <c r="AH23" s="18">
+        <f>'[8]Financial Model'!$Y$24</f>
+        <v>-4.8380647740903671E-2</v>
+      </c>
+      <c r="AJ23" s="18">
+        <f>'[8]Financial Model'!$AI$24</f>
+        <v>-2.7349948660505885E-2</v>
+      </c>
+      <c r="AK23" s="18">
+        <f>'[8]Financial Model'!$AH$24</f>
+        <v>0.17018022938285093</v>
+      </c>
+      <c r="AL23" s="18">
+        <f>'[8]Financial Model'!$AG$24</f>
+        <v>-0.14805509026614549</v>
+      </c>
+      <c r="AM23" s="18">
+        <f>'[8]Financial Model'!$AF$24</f>
+        <v>8.2502266545784186E-2</v>
+      </c>
+      <c r="AO23" s="5">
         <f>[8]Main!$C$24</f>
         <v>1995</v>
       </c>
-      <c r="AI23" s="5">
+      <c r="AP23" s="5">
         <f>[8]Main!$C$25</f>
         <v>1998</v>
       </c>
-      <c r="AJ23" s="5" t="str">
+      <c r="AQ23" s="5" t="str">
         <f>[8]Main!$C$23</f>
         <v>San Jose, CA</v>
       </c>
-      <c r="AL23" s="5" t="s">
+      <c r="AS23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM23" s="5" t="s">
+      <c r="AT23" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -3254,14 +3439,14 @@
       <c r="E24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AL24" s="5" t="s">
+      <c r="AS24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM24" s="5" t="s">
+      <c r="AT24" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
@@ -3274,12 +3459,12 @@
       <c r="E25" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AL25" s="5" t="s">
+      <c r="AS25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM25" s="5"/>
-    </row>
-    <row r="26" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT25" s="5"/>
+    </row>
+    <row r="26" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
@@ -3289,12 +3474,12 @@
       <c r="D26" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AL26" s="5" t="s">
+      <c r="AS26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM26" s="5"/>
-    </row>
-    <row r="27" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT26" s="5"/>
+    </row>
+    <row r="27" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
@@ -3304,9 +3489,9 @@
       <c r="D27" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="AM27" s="5"/>
-    </row>
-    <row r="30" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT27" s="5"/>
+    </row>
+    <row r="30" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -3319,11 +3504,11 @@
       <c r="E30" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="AL30" s="5" t="s">
+      <c r="AS30" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3336,11 +3521,11 @@
       <c r="E31" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AL31" s="5" t="s">
+      <c r="AS31" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>106</v>
       </c>
@@ -3350,14 +3535,14 @@
       <c r="D34" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AL34" s="5" t="s">
+      <c r="AS34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM34" s="5" t="s">
+      <c r="AT34" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>108</v>
       </c>
@@ -3373,14 +3558,14 @@
       <c r="U35" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="AL35" s="5" t="s">
+      <c r="AS35" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM35" s="5" t="s">
+      <c r="AT35" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>110</v>
       </c>
@@ -3390,14 +3575,14 @@
       <c r="D36" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="AL36" s="5" t="s">
+      <c r="AS36" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AM36" s="5" t="s">
+      <c r="AT36" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="39" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3420,33 +3605,33 @@
         <f>G39*F39</f>
         <v>482.83839999999998</v>
       </c>
-      <c r="AH39" s="5">
+      <c r="AO39" s="5">
         <v>2007</v>
       </c>
-      <c r="AI39" s="5">
+      <c r="AP39" s="5">
         <v>2021</v>
       </c>
-      <c r="AJ39" s="5" t="s">
+      <c r="AQ39" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AL39" s="5" t="s">
+      <c r="AS39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AM39" s="5" t="s">
+      <c r="AT39" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.2">
       <c r="G40" s="19"/>
       <c r="H40" s="17"/>
-      <c r="AM40" s="5"/>
-    </row>
-    <row r="41" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT40" s="5"/>
+    </row>
+    <row r="41" spans="2:46" x14ac:dyDescent="0.2">
       <c r="G41" s="19"/>
       <c r="H41" s="17"/>
-      <c r="AM41" s="5"/>
-    </row>
-    <row r="42" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT41" s="5"/>
+    </row>
+    <row r="42" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>121</v>
       </c>
@@ -3470,14 +3655,14 @@
         <f>G42*F42</f>
         <v>122932.59181199998</v>
       </c>
-      <c r="AL42" s="5" t="s">
+      <c r="AS42" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AM42" s="5" t="s">
+      <c r="AT42" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
@@ -3501,14 +3686,14 @@
         <f>G43*F43</f>
         <v>14757.024674</v>
       </c>
-      <c r="AL43" s="5" t="s">
+      <c r="AS43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AM43" s="5" t="s">
+      <c r="AT43" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
@@ -3531,19 +3716,19 @@
         <f>G44*F44</f>
         <v>65.118500000000012</v>
       </c>
-      <c r="AL44" s="5" t="s">
+      <c r="AS44" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AM44" s="5" t="s">
+      <c r="AT44" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="2:39" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:46" x14ac:dyDescent="0.2">
       <c r="G45" s="19"/>
       <c r="H45" s="17"/>
-      <c r="AM45" s="5"/>
-    </row>
-    <row r="46" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT45" s="5"/>
+    </row>
+    <row r="46" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
@@ -3552,9 +3737,9 @@
       </c>
       <c r="G46" s="19"/>
       <c r="H46" s="17"/>
-      <c r="AM46" s="5"/>
-    </row>
-    <row r="47" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT46" s="5"/>
+    </row>
+    <row r="47" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
@@ -3563,9 +3748,9 @@
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="17"/>
-      <c r="AM47" s="5"/>
-    </row>
-    <row r="48" spans="2:39" x14ac:dyDescent="0.15">
+      <c r="AT47" s="5"/>
+    </row>
+    <row r="48" spans="2:46" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
@@ -3574,14 +3759,14 @@
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="17"/>
-      <c r="AM48" s="5"/>
-    </row>
-    <row r="49" spans="5:39" x14ac:dyDescent="0.15">
+      <c r="AT48" s="5"/>
+    </row>
+    <row r="49" spans="5:46" x14ac:dyDescent="0.2">
       <c r="G49" s="19"/>
       <c r="H49" s="17"/>
-      <c r="AM49" s="5"/>
-    </row>
-    <row r="53" spans="5:39" x14ac:dyDescent="0.15">
+      <c r="AT49" s="5"/>
+    </row>
+    <row r="53" spans="5:46" x14ac:dyDescent="0.2">
       <c r="E53" s="33" t="s">
         <v>25</v>
       </c>
@@ -3590,7 +3775,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="5:39" x14ac:dyDescent="0.15">
+    <row r="54" spans="5:46" x14ac:dyDescent="0.2">
       <c r="E54" s="10" t="s">
         <v>27</v>
       </c>
@@ -3602,7 +3787,7 @@
         <v>1.2048192771084338</v>
       </c>
     </row>
-    <row r="55" spans="5:39" x14ac:dyDescent="0.15">
+    <row r="55" spans="5:46" x14ac:dyDescent="0.2">
       <c r="E55" s="13" t="s">
         <v>28</v>
       </c>
@@ -3646,21 +3831,21 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.1640625" style="1"/>
+    <col min="4" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -3693,7 +3878,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -3719,11 +3904,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Start basic $GOOG model
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9883D75B-8360-4829-BBC9-DB7ED81297B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A1E57E-B644-4289-ABB4-C58873A81935}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
@@ -27,6 +27,7 @@
     <externalReference r:id="rId10"/>
     <externalReference r:id="rId11"/>
     <externalReference r:id="rId12"/>
+    <externalReference r:id="rId13"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="161">
   <si>
     <t>Ticker</t>
   </si>
@@ -518,6 +519,9 @@
   </si>
   <si>
     <t>Hardware, Services</t>
+  </si>
+  <si>
+    <t>Alphabet Inc.</t>
   </si>
 </sst>
 </file>
@@ -840,6 +844,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -849,7 +854,6 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -989,6 +993,62 @@
           </cell>
         </row>
       </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink10.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Main"/>
+      <sheetName val="Financial Model"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="6">
+          <cell r="C6">
+            <v>95.46</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="C7">
+            <v>13523</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="C8">
+            <v>1290905.5799999998</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="C11">
+            <v>0</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="C12">
+            <v>1290905.5799999998</v>
+          </cell>
+        </row>
+        <row r="23">
+          <cell r="C23" t="str">
+            <v>Mountain View, CA</v>
+          </cell>
+        </row>
+        <row r="24">
+          <cell r="C24">
+            <v>1998</v>
+          </cell>
+        </row>
+        <row r="25">
+          <cell r="C25">
+            <v>2004</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2216,10 +2276,10 @@
   <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="Y21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M51" sqref="M51"/>
+      <selection pane="bottomRight" activeCell="AQ53" sqref="AQ53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2252,20 +2312,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="W1" s="36" t="s">
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+      <c r="J1" s="37"/>
+      <c r="W1" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
+      <c r="X1" s="37"/>
+      <c r="Y1" s="37"/>
+      <c r="Z1" s="37"/>
+      <c r="AA1" s="37"/>
       <c r="AB1" s="5"/>
     </row>
     <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
@@ -3873,19 +3933,19 @@
         <f>[9]Main!$C$6*$F$57</f>
         <v>213.21039999999999</v>
       </c>
-      <c r="G51" s="37">
+      <c r="G51" s="34">
         <f>[9]Main!$C$7</f>
         <v>7440</v>
       </c>
-      <c r="H51" s="37">
+      <c r="H51" s="34">
         <f>[9]Main!$C$12*$F$57</f>
         <v>1586285.3759999999</v>
       </c>
-      <c r="I51" s="37">
+      <c r="I51" s="34">
         <f>[9]Main!$C$11*$F$57</f>
         <v>0</v>
       </c>
-      <c r="J51" s="37">
+      <c r="J51" s="34">
         <f>[9]Main!$C$12*$F$57</f>
         <v>1586285.3759999999</v>
       </c>
@@ -3917,11 +3977,57 @@
       </c>
     </row>
     <row r="52" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="7" t="s">
         <v>151</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="E52" s="5" t="s">
         <v>17</v>
+      </c>
+      <c r="F52" s="16">
+        <f>[10]Main!$C$6*$F$57</f>
+        <v>79.231799999999993</v>
+      </c>
+      <c r="G52" s="34">
+        <f>[10]Main!$C$7</f>
+        <v>13523</v>
+      </c>
+      <c r="H52" s="34">
+        <f>[10]Main!$C$8*$F$57</f>
+        <v>1071451.6313999998</v>
+      </c>
+      <c r="I52" s="34">
+        <f>[10]Main!$C$11*$F$57</f>
+        <v>0</v>
+      </c>
+      <c r="J52" s="34">
+        <f>[10]Main!$C$12*$F$57</f>
+        <v>1071451.6313999998</v>
+      </c>
+      <c r="K52" s="5">
+        <f>[10]Main!$C$28</f>
+        <v>0</v>
+      </c>
+      <c r="L52" s="5">
+        <f>[10]Main!$D$28</f>
+        <v>0</v>
+      </c>
+      <c r="AO52" s="5">
+        <f>[10]Main!$C$24</f>
+        <v>1998</v>
+      </c>
+      <c r="AP52" s="5">
+        <f>[10]Main!$C$25</f>
+        <v>2004</v>
+      </c>
+      <c r="AQ52" s="5" t="str">
+        <f>[10]Main!$C$23</f>
+        <v>Mountain View, CA</v>
       </c>
       <c r="AS52" s="5" t="s">
         <v>156</v>
@@ -3959,10 +4065,10 @@
       </c>
     </row>
     <row r="56" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="E56" s="34" t="s">
+      <c r="E56" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="35"/>
+      <c r="F56" s="36"/>
       <c r="G56" s="9" t="s">
         <v>26</v>
       </c>
@@ -4007,9 +4113,10 @@
     <hyperlink ref="B20" r:id="rId7" xr:uid="{B9C2E740-5539-4983-8CC4-F329408A4445}"/>
     <hyperlink ref="B22" r:id="rId8" xr:uid="{03436A82-476B-4BF2-A855-FEC5F745CF98}"/>
     <hyperlink ref="B51" r:id="rId9" xr:uid="{46DC7469-9CFC-4610-A22B-3D4E075DFC99}"/>
+    <hyperlink ref="B52" r:id="rId10" xr:uid="{1F04985A-EB8E-4ED3-BC5F-B6E427A61566}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId10"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId11"/>
   <ignoredErrors>
     <ignoredError sqref="I51" formula="1"/>
   </ignoredErrors>

</xml_diff>

<commit_message>
$RBLX Q422 earnings release
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14A1E57E-B644-4289-ABB4-C58873A81935}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAEAF9C-7877-4755-9059-9BF2A88F0253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
@@ -1047,6 +1047,10 @@
             <v>2004</v>
           </cell>
         </row>
+        <row r="28">
+          <cell r="C28"/>
+          <cell r="D28"/>
+        </row>
       </sheetData>
       <sheetData sheetId="1"/>
     </sheetDataSet>
@@ -1469,7 +1473,7 @@
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>37.21</v>
+            <v>41.46</v>
           </cell>
           <cell r="G6" t="str">
             <v>San Mateo, CA</v>
@@ -1477,7 +1481,7 @@
         </row>
         <row r="7">
           <cell r="C7">
-            <v>597.779</v>
+            <v>601.85900000000004</v>
           </cell>
           <cell r="G7">
             <v>2021</v>
@@ -1485,7 +1489,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>22243.356589999999</v>
+            <v>24953.074140000001</v>
           </cell>
           <cell r="G8">
             <v>2004</v>
@@ -1493,26 +1497,28 @@
         </row>
         <row r="11">
           <cell r="C11">
-            <v>2032.8440000000001</v>
+            <v>1988.4900000000002</v>
           </cell>
           <cell r="G11" t="str">
-            <v>Q322</v>
-          </cell>
-          <cell r="H11"/>
+            <v>Q422</v>
+          </cell>
+          <cell r="H11">
+            <v>42036</v>
+          </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>20210.512589999998</v>
+            <v>22964.584140000003</v>
           </cell>
         </row>
         <row r="16">
           <cell r="G16">
-            <v>52.387601721181568</v>
+            <v>81.803970495189361</v>
           </cell>
         </row>
         <row r="17">
           <cell r="G17">
-            <v>11.590025427513091</v>
+            <v>11.214602687937182</v>
           </cell>
         </row>
       </sheetData>
@@ -1550,7 +1556,7 @@
         </row>
         <row r="26">
           <cell r="AP26">
-            <v>66.171403527895578</v>
+            <v>64.111668818778071</v>
           </cell>
         </row>
         <row r="28">
@@ -1561,7 +1567,7 @@
             <v>1.0772942519902369</v>
           </cell>
           <cell r="AP28">
-            <v>0.77832312625357636</v>
+            <v>0.54634994738972664</v>
           </cell>
         </row>
       </sheetData>
@@ -1948,6 +1954,10 @@
           <cell r="C25">
             <v>1986</v>
           </cell>
+        </row>
+        <row r="29">
+          <cell r="C29"/>
+          <cell r="D29"/>
         </row>
       </sheetData>
       <sheetData sheetId="1"/>
@@ -2276,10 +2286,10 @@
   <dimension ref="A1:AT58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="Y21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AQ53" sqref="AQ53"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3153,39 +3163,39 @@
       </c>
       <c r="F19" s="17">
         <f>[5]Main!$C$6*F57</f>
-        <v>30.8843</v>
+        <v>34.411799999999999</v>
       </c>
       <c r="G19" s="17">
         <f>[5]Main!$C$7</f>
-        <v>597.779</v>
+        <v>601.85900000000004</v>
       </c>
       <c r="H19" s="17">
         <f>[5]Main!$C$8*F57</f>
-        <v>18461.985969699999</v>
+        <v>20711.051536200001</v>
       </c>
       <c r="I19" s="17">
         <f>[5]Main!$C$11*F57</f>
-        <v>1687.26052</v>
+        <v>1650.4467000000002</v>
       </c>
       <c r="J19" s="17">
         <f>[5]Main!$C$12*F57</f>
-        <v>16774.725449699999</v>
+        <v>19060.6048362</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>[5]Main!$G$11</f>
-        <v>Q322</v>
-      </c>
-      <c r="L19" s="5">
+        <v>Q422</v>
+      </c>
+      <c r="L19" s="8">
         <f>[5]Main!$H$11</f>
-        <v>0</v>
+        <v>42036</v>
       </c>
       <c r="M19" s="27">
         <f>'[5]Financial Model'!$AP$26*F57</f>
-        <v>54.922264928153325</v>
+        <v>53.212685119585799</v>
       </c>
       <c r="N19" s="32">
         <f>'[5]Financial Model'!$AP$28</f>
-        <v>0.77832312625357636</v>
+        <v>0.54634994738972664</v>
       </c>
       <c r="O19" s="32">
         <f>'[5]Financial Model'!$AP$22</f>
@@ -3193,11 +3203,11 @@
       </c>
       <c r="Q19" s="21">
         <f>[5]Main!$G$16</f>
-        <v>52.387601721181568</v>
+        <v>81.803970495189361</v>
       </c>
       <c r="R19" s="21">
         <f>[5]Main!$G$17</f>
-        <v>11.590025427513091</v>
+        <v>11.214602687937182</v>
       </c>
       <c r="X19" s="25">
         <f>'[5]Financial Model'!$W$18*F57</f>

</xml_diff>

<commit_message>
$EBAY Q4/FY 22 results
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F69B63DD-CF82-4347-94ED-33DC8C9818D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625DF4B-E277-694F-AB79-974128A2F4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener" sheetId="2" r:id="rId1"/>
@@ -33,6 +33,16 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -842,12 +852,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="17" fontId="1" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -855,6 +859,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1801,32 +1811,33 @@
     <sheetNames>
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
+      <sheetName val="Historical Projections"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>49.5</v>
+            <v>45.35</v>
           </cell>
         </row>
         <row r="7">
           <cell r="C7">
-            <v>542.659087</v>
+            <v>541</v>
           </cell>
         </row>
         <row r="8">
           <cell r="C8">
-            <v>26861.6248065</v>
+            <v>24534.350000000002</v>
           </cell>
         </row>
         <row r="11">
           <cell r="C11">
-            <v>-4235</v>
+            <v>-4092</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>31096.6248065</v>
+            <v>28626.350000000002</v>
           </cell>
         </row>
         <row r="23">
@@ -1846,35 +1857,35 @@
         </row>
         <row r="28">
           <cell r="C28" t="str">
-            <v>Q322</v>
+            <v>Q422</v>
           </cell>
           <cell r="D28">
-            <v>37561</v>
+            <v>44593</v>
           </cell>
         </row>
         <row r="33">
           <cell r="C33">
-            <v>5.5350555958170204</v>
+            <v>5.071005480208119</v>
           </cell>
         </row>
         <row r="34">
           <cell r="C34">
-            <v>2.7138436862497475</v>
+            <v>2.4787179228126894</v>
           </cell>
         </row>
         <row r="35">
           <cell r="C35">
-            <v>3.1417079012426754</v>
+            <v>2.8921347747019603</v>
           </cell>
         </row>
         <row r="36">
           <cell r="C36">
-            <v>-421.2402023888468</v>
+            <v>-385.92410461281213</v>
           </cell>
         </row>
         <row r="37">
           <cell r="C37">
-            <v>1110.5937430892857</v>
+            <v>1022.3696428571429</v>
           </cell>
         </row>
       </sheetData>
@@ -1889,10 +1900,13 @@
           <cell r="AE20">
             <v>-1347</v>
           </cell>
+          <cell r="AJ20">
+            <v>-1268.75</v>
+          </cell>
         </row>
         <row r="24">
-          <cell r="Y24">
-            <v>-4.8380647740903671E-2</v>
+          <cell r="Z24">
+            <v>-3.9418293149636408E-2</v>
           </cell>
           <cell r="AF24">
             <v>8.2502266545784186E-2</v>
@@ -1905,6 +1919,9 @@
           </cell>
           <cell r="AI24">
             <v>-2.7349948660505885E-2</v>
+          </cell>
+          <cell r="AJ24">
+            <v>-5.9980806142034604E-2</v>
           </cell>
         </row>
         <row r="25">
@@ -1913,34 +1930,35 @@
           </cell>
         </row>
         <row r="27">
-          <cell r="U27">
-            <v>0.72890843662534988</v>
+          <cell r="Z27">
+            <v>0.72868525896414338</v>
           </cell>
         </row>
         <row r="28">
-          <cell r="U28">
-            <v>0.2646941223510596</v>
+          <cell r="Z28">
+            <v>0.22519920318725101</v>
           </cell>
         </row>
         <row r="29">
-          <cell r="U29">
-            <v>0.10555777688924431</v>
+          <cell r="Z29">
+            <v>0.26782868525896414</v>
           </cell>
           <cell r="AW29">
-            <v>57.281112716189718</v>
+            <v>59.008797946830612</v>
           </cell>
         </row>
         <row r="30">
-          <cell r="U30">
-            <v>0.34792626728110598</v>
+          <cell r="Z30">
+            <v>0.19053361471208924</v>
           </cell>
         </row>
         <row r="31">
           <cell r="AW31">
-            <v>0.15719419628666098</v>
+            <v>0.30118628328182151</v>
           </cell>
         </row>
       </sheetData>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2307,9 +2325,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2324,56 +2342,56 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="P23" sqref="P22:P23"/>
+      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="5"/>
-    <col min="6" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="5"/>
-    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" style="26" customWidth="1"/>
-    <col min="14" max="15" width="9.42578125" style="27" customWidth="1"/>
-    <col min="16" max="23" width="9.42578125" style="5" customWidth="1"/>
-    <col min="24" max="27" width="9.42578125" style="22" customWidth="1"/>
-    <col min="28" max="28" width="9.140625" style="1"/>
-    <col min="29" max="32" width="9.140625" style="5"/>
-    <col min="33" max="33" width="9.140625" style="1"/>
-    <col min="34" max="39" width="9.140625" style="18"/>
-    <col min="40" max="40" width="9.140625" style="1"/>
-    <col min="41" max="42" width="9.140625" style="5"/>
+    <col min="4" max="5" width="9.1640625" style="5"/>
+    <col min="6" max="7" width="9.1640625" style="1"/>
+    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="1"/>
+    <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1640625" style="5"/>
+    <col min="12" max="12" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5" style="26" customWidth="1"/>
+    <col min="14" max="15" width="9.5" style="27" customWidth="1"/>
+    <col min="16" max="23" width="9.5" style="5" customWidth="1"/>
+    <col min="24" max="27" width="9.5" style="22" customWidth="1"/>
+    <col min="28" max="28" width="9.1640625" style="1"/>
+    <col min="29" max="32" width="9.1640625" style="5"/>
+    <col min="33" max="33" width="9.1640625" style="1"/>
+    <col min="34" max="39" width="9.1640625" style="18"/>
+    <col min="40" max="40" width="9.1640625" style="1"/>
+    <col min="41" max="42" width="9.1640625" style="5"/>
     <col min="43" max="43" width="21" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.140625" style="1"/>
-    <col min="45" max="45" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="9.1640625" style="1"/>
+    <col min="45" max="45" width="17.5" style="5" bestFit="1" customWidth="1"/>
     <col min="46" max="46" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.140625" style="1"/>
+    <col min="47" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="38" t="s">
+    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F1" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="W1" s="38" t="s">
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="W1" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2496,7 +2514,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.15">
       <c r="F3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -2507,7 +2525,7 @@
       <c r="AA3" s="23"/>
       <c r="AT3" s="5"/>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
@@ -2627,7 +2645,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B5" s="7" t="s">
         <v>80</v>
       </c>
@@ -2724,7 +2742,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
       <c r="F6" s="16"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -2739,7 +2757,7 @@
       <c r="AA6" s="23"/>
       <c r="AT6" s="5"/>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2889,7 +2907,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B8" s="7"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
@@ -2917,7 +2935,7 @@
       <c r="AF8" s="18"/>
       <c r="AT8" s="5"/>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2943,7 +2961,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2965,7 +2983,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -3115,13 +3133,13 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B12" s="7"/>
       <c r="F12" s="16"/>
       <c r="W12" s="22"/>
       <c r="AT12" s="5"/>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
@@ -3152,10 +3170,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.15">
       <c r="W14" s="22"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -3176,7 +3194,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
@@ -3197,13 +3215,13 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W17" s="22"/>
     </row>
-    <row r="18" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W18" s="22"/>
     </row>
-    <row r="19" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
@@ -3337,7 +3355,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3386,10 +3404,10 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W21" s="22"/>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
@@ -3517,7 +3535,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B23" s="7" t="s">
         <v>82</v>
       </c>
@@ -3532,39 +3550,39 @@
       </c>
       <c r="F23" s="16">
         <f>[8]Main!$C$6*F57</f>
-        <v>41.085000000000001</v>
+        <v>37.640499999999996</v>
       </c>
       <c r="G23" s="19">
         <f>[8]Main!$C$7</f>
-        <v>542.659087</v>
+        <v>541</v>
       </c>
       <c r="H23" s="17">
         <f>[8]Main!$C$8*F57</f>
-        <v>22295.148589394998</v>
+        <v>20363.5105</v>
       </c>
       <c r="I23" s="17">
         <f>[8]Main!$C$11*F57</f>
-        <v>-3515.0499999999997</v>
+        <v>-3396.3599999999997</v>
       </c>
       <c r="J23" s="17">
         <f>[8]Main!$C$12*F57</f>
-        <v>25810.198589395</v>
-      </c>
-      <c r="K23" s="25" t="str">
+        <v>23759.870500000001</v>
+      </c>
+      <c r="K23" s="37" t="str">
         <f>[8]Main!$C$28</f>
-        <v>Q322</v>
-      </c>
-      <c r="L23" s="35">
+        <v>Q422</v>
+      </c>
+      <c r="L23" s="38">
         <f>[8]Main!$D$28</f>
-        <v>37561</v>
+        <v>44593</v>
       </c>
       <c r="M23" s="26">
         <f>'[8]Financial Model'!$AW$29*$F$57</f>
-        <v>47.543323554437464</v>
+        <v>48.977302295869407</v>
       </c>
       <c r="N23" s="31">
         <f>'[8]Financial Model'!$AW$31</f>
-        <v>0.15719419628666098</v>
+        <v>0.30118628328182151</v>
       </c>
       <c r="O23" s="31">
         <f>'[8]Financial Model'!$AW$25</f>
@@ -3573,26 +3591,29 @@
       <c r="P23" s="8"/>
       <c r="Q23" s="21">
         <f>[8]Main!$C$33</f>
-        <v>5.5350555958170204</v>
+        <v>5.071005480208119</v>
       </c>
       <c r="R23" s="21">
         <f>[8]Main!$C$34</f>
-        <v>2.7138436862497475</v>
+        <v>2.4787179228126894</v>
       </c>
       <c r="S23" s="21">
         <f>[8]Main!$C$35</f>
-        <v>3.1417079012426754</v>
+        <v>2.8921347747019603</v>
       </c>
       <c r="T23" s="21">
         <f>[8]Main!$C$36</f>
-        <v>-421.2402023888468</v>
+        <v>-385.92410461281213</v>
       </c>
       <c r="U23" s="21">
         <f>[8]Main!$C$37</f>
-        <v>1110.5937430892857</v>
+        <v>1022.3696428571429</v>
       </c>
       <c r="V23" s="8"/>
-      <c r="W23" s="34"/>
+      <c r="W23" s="24">
+        <f>'[8]Financial Model'!$AJ$20*F57</f>
+        <v>-1053.0625</v>
+      </c>
       <c r="X23" s="24">
         <f>'[8]Financial Model'!$AE$20*F57</f>
         <v>-1118.01</v>
@@ -3610,24 +3631,28 @@
         <v>2078.3132530120483</v>
       </c>
       <c r="AC23" s="18">
-        <f>'[8]Financial Model'!$U$27</f>
-        <v>0.72890843662534988</v>
+        <f>'[8]Financial Model'!$Z$27</f>
+        <v>0.72868525896414338</v>
       </c>
       <c r="AD23" s="18">
-        <f>'[8]Financial Model'!$U$28</f>
-        <v>0.2646941223510596</v>
+        <f>'[8]Financial Model'!$Z$28</f>
+        <v>0.22519920318725101</v>
       </c>
       <c r="AE23" s="18">
-        <f>'[8]Financial Model'!$U$29</f>
-        <v>0.10555777688924431</v>
+        <f>'[8]Financial Model'!$Z$29</f>
+        <v>0.26782868525896414</v>
       </c>
       <c r="AF23" s="18">
-        <f>'[8]Financial Model'!$U$30</f>
-        <v>0.34792626728110598</v>
+        <f>'[8]Financial Model'!$Z$30</f>
+        <v>0.19053361471208924</v>
       </c>
       <c r="AH23" s="18">
-        <f>'[8]Financial Model'!$Y$24</f>
-        <v>-4.8380647740903671E-2</v>
+        <f>'[8]Financial Model'!$Z$24</f>
+        <v>-3.9418293149636408E-2</v>
+      </c>
+      <c r="AI23" s="18">
+        <f>'[8]Financial Model'!$AJ$24</f>
+        <v>-5.9980806142034604E-2</v>
       </c>
       <c r="AJ23" s="18">
         <f>'[8]Financial Model'!$AI$24</f>
@@ -3664,7 +3689,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -3685,7 +3710,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
@@ -3704,7 +3729,7 @@
       </c>
       <c r="AT25" s="5"/>
     </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
@@ -3720,7 +3745,7 @@
       </c>
       <c r="AT26" s="5"/>
     </row>
-    <row r="27" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
@@ -3733,13 +3758,13 @@
       <c r="W27" s="22"/>
       <c r="AT27" s="5"/>
     </row>
-    <row r="28" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W28" s="22"/>
     </row>
-    <row r="29" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W29" s="22"/>
     </row>
-    <row r="30" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -3757,7 +3782,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3775,13 +3800,13 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W32" s="22"/>
     </row>
-    <row r="33" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W33" s="22"/>
     </row>
-    <row r="34" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
         <v>106</v>
       </c>
@@ -3799,7 +3824,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
         <v>108</v>
       </c>
@@ -3823,7 +3848,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
         <v>110</v>
       </c>
@@ -3841,13 +3866,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W37" s="22"/>
     </row>
-    <row r="38" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:46" x14ac:dyDescent="0.15">
       <c r="W38" s="22"/>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3887,19 +3912,19 @@
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:46" x14ac:dyDescent="0.15">
       <c r="G40" s="19"/>
       <c r="H40" s="17"/>
       <c r="W40" s="22"/>
       <c r="AT40" s="5"/>
     </row>
-    <row r="41" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:46" x14ac:dyDescent="0.15">
       <c r="G41" s="19"/>
       <c r="H41" s="17"/>
       <c r="W41" s="22"/>
       <c r="AT41" s="5"/>
     </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
         <v>121</v>
       </c>
@@ -3931,7 +3956,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
@@ -3963,7 +3988,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
@@ -3994,13 +4019,13 @@
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:46" x14ac:dyDescent="0.15">
       <c r="G45" s="19"/>
       <c r="H45" s="17"/>
       <c r="W45" s="22"/>
       <c r="AT45" s="5"/>
     </row>
-    <row r="46" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
@@ -4012,7 +4037,7 @@
       <c r="W46" s="22"/>
       <c r="AT46" s="5"/>
     </row>
-    <row r="47" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
@@ -4024,7 +4049,7 @@
       <c r="W47" s="22"/>
       <c r="AT47" s="5"/>
     </row>
-    <row r="48" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
@@ -4036,19 +4061,19 @@
       <c r="W48" s="22"/>
       <c r="AT48" s="5"/>
     </row>
-    <row r="49" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:46" x14ac:dyDescent="0.15">
       <c r="G49" s="19"/>
       <c r="H49" s="17"/>
       <c r="W49" s="22"/>
       <c r="AT49" s="5"/>
     </row>
-    <row r="50" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:46" x14ac:dyDescent="0.15">
       <c r="G50" s="19"/>
       <c r="H50" s="17"/>
       <c r="W50" s="22"/>
       <c r="AT50" s="5"/>
     </row>
-    <row r="51" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B51" s="7" t="s">
         <v>150</v>
       </c>
@@ -4109,7 +4134,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B52" s="7" t="s">
         <v>151</v>
       </c>
@@ -4170,7 +4195,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
         <v>152</v>
       </c>
@@ -4184,7 +4209,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B54" s="1" t="s">
         <v>153</v>
       </c>
@@ -4198,16 +4223,16 @@
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="2:46" x14ac:dyDescent="0.2">
-      <c r="E56" s="36" t="s">
+    <row r="56" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="E56" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="37"/>
+      <c r="F56" s="35"/>
       <c r="G56" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="57" spans="2:46" x14ac:dyDescent="0.15">
       <c r="E57" s="10" t="s">
         <v>27</v>
       </c>
@@ -4219,7 +4244,7 @@
         <v>1.2048192771084338</v>
       </c>
     </row>
-    <row r="58" spans="2:46" x14ac:dyDescent="0.2">
+    <row r="58" spans="2:46" x14ac:dyDescent="0.15">
       <c r="E58" s="13" t="s">
         <v>28</v>
       </c>
@@ -4268,21 +4293,21 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1640625" style="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.140625" style="1"/>
+    <col min="4" max="8" width="9.1640625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="1"/>
+    <col min="14" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4315,7 +4340,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -4341,11 +4366,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Employee Count added to Software Overview & $RBLX
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Stocks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6625DF4B-E277-694F-AB79-974128A2F4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C0D0B0-47B1-4E43-9EFE-BF69CA09436A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
+    <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18900" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Screener" sheetId="2" r:id="rId1"/>
@@ -34,22 +34,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="162">
   <si>
     <t>Ticker</t>
   </si>
@@ -532,6 +522,9 @@
   </si>
   <si>
     <t>Alphabet Inc.</t>
+  </si>
+  <si>
+    <t>Employees</t>
   </si>
 </sst>
 </file>
@@ -769,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -852,6 +845,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -861,10 +860,10 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1516,6 +1515,11 @@
             <v>2004</v>
           </cell>
         </row>
+        <row r="10">
+          <cell r="G10">
+            <v>2128</v>
+          </cell>
+        </row>
         <row r="11">
           <cell r="C11">
             <v>1988.4900000000002</v>
@@ -1926,7 +1930,7 @@
         </row>
         <row r="25">
           <cell r="AW25">
-            <v>0.08</v>
+            <v>0.09</v>
           </cell>
         </row>
         <row r="27">
@@ -1944,7 +1948,7 @@
             <v>0.26782868525896414</v>
           </cell>
           <cell r="AW29">
-            <v>59.008797946830612</v>
+            <v>53.181611591692423</v>
           </cell>
         </row>
         <row r="30">
@@ -1954,7 +1958,7 @@
         </row>
         <row r="31">
           <cell r="AW31">
-            <v>0.30118628328182151</v>
+            <v>0.17269264810788143</v>
           </cell>
         </row>
       </sheetData>
@@ -2325,9 +2329,9 @@
       <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2336,62 +2340,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1873CD5B-C727-4CC0-ACC4-210B76523995}">
-  <dimension ref="A1:AT58"/>
+  <dimension ref="A1:AU58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="O3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="AO20" sqref="AO20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="23" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="5"/>
-    <col min="6" max="7" width="9.1640625" style="1"/>
-    <col min="8" max="8" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="1"/>
-    <col min="10" max="10" width="9.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1640625" style="5"/>
-    <col min="12" max="12" width="9.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5" style="26" customWidth="1"/>
-    <col min="14" max="15" width="9.5" style="27" customWidth="1"/>
-    <col min="16" max="23" width="9.5" style="5" customWidth="1"/>
-    <col min="24" max="27" width="9.5" style="22" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" style="1"/>
-    <col min="29" max="32" width="9.1640625" style="5"/>
-    <col min="33" max="33" width="9.1640625" style="1"/>
-    <col min="34" max="39" width="9.1640625" style="18"/>
-    <col min="40" max="40" width="9.1640625" style="1"/>
-    <col min="41" max="42" width="9.1640625" style="5"/>
-    <col min="43" max="43" width="21" style="5" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="9.1640625" style="1"/>
-    <col min="45" max="45" width="17.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="30" style="1" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.1640625" style="1"/>
+    <col min="4" max="5" width="9.140625" style="5"/>
+    <col min="6" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="5"/>
+    <col min="12" max="12" width="9.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="26" customWidth="1"/>
+    <col min="14" max="15" width="9.42578125" style="27" customWidth="1"/>
+    <col min="16" max="23" width="9.42578125" style="5" customWidth="1"/>
+    <col min="24" max="27" width="9.42578125" style="22" customWidth="1"/>
+    <col min="28" max="28" width="9.140625" style="1"/>
+    <col min="29" max="32" width="9.140625" style="5"/>
+    <col min="33" max="33" width="9.140625" style="1"/>
+    <col min="34" max="39" width="9.140625" style="18"/>
+    <col min="40" max="40" width="9.140625" style="1"/>
+    <col min="41" max="41" width="11.28515625" style="39" bestFit="1" customWidth="1"/>
+    <col min="42" max="43" width="9.140625" style="5"/>
+    <col min="44" max="44" width="21" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="9.140625" style="1"/>
+    <col min="46" max="46" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="30" style="1" bestFit="1" customWidth="1"/>
+    <col min="48" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="F1" s="36" t="s">
+    <row r="1" spans="1:47" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="W1" s="36" t="s">
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="W1" s="38" t="s">
         <v>105</v>
       </c>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
       <c r="AB1" s="5"/>
     </row>
-    <row r="2" spans="1:46" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:47" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -2498,23 +2503,26 @@
       <c r="AM2" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AO2" s="40" t="s">
+        <v>161</v>
+      </c>
+      <c r="AP2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AS2" s="4" t="s">
+      <c r="AT2" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AT2" s="4" t="s">
+      <c r="AU2" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:47" x14ac:dyDescent="0.2">
       <c r="F3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="17"/>
@@ -2523,9 +2531,9 @@
       <c r="Y3" s="23"/>
       <c r="Z3" s="23"/>
       <c r="AA3" s="23"/>
-      <c r="AT3" s="5"/>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.15">
+      <c r="AU3" s="5"/>
+    </row>
+    <row r="4" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B4" s="7" t="s">
         <v>32</v>
       </c>
@@ -2626,26 +2634,26 @@
         <f>'[1]Financial Model'!$AH$26</f>
         <v>0.48003319895660423</v>
       </c>
-      <c r="AO4" s="5">
+      <c r="AP4" s="5">
         <f>[1]Main!$C24</f>
         <v>2007</v>
       </c>
-      <c r="AP4" s="5">
+      <c r="AQ4" s="5">
         <f>[1]Main!$C$25</f>
         <v>2017</v>
       </c>
-      <c r="AQ4" s="5" t="str">
+      <c r="AR4" s="5" t="str">
         <f>[1]Main!$C$23</f>
         <v>New York City, NY</v>
       </c>
-      <c r="AS4" s="5" t="s">
+      <c r="AT4" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AT4" s="5" t="s">
+      <c r="AU4" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>80</v>
       </c>
@@ -2723,26 +2731,26 @@
         <f>'[2]Financial Model'!$J$25</f>
         <v>0.21252241299870667</v>
       </c>
-      <c r="AO5" s="5">
+      <c r="AP5" s="5">
         <f>[2]Main!$C$24</f>
         <v>2010</v>
       </c>
-      <c r="AP5" s="5">
+      <c r="AQ5" s="5">
         <f>[2]Main!$C$25</f>
         <v>2022</v>
       </c>
-      <c r="AQ5" s="5" t="str">
+      <c r="AR5" s="5" t="str">
         <f>[2]Main!$C$23</f>
         <v>Redwood City, CA</v>
       </c>
-      <c r="AS5" s="5" t="s">
+      <c r="AT5" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AT5" s="5" t="s">
+      <c r="AU5" s="5" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.2">
       <c r="F6" s="16"/>
       <c r="I6" s="17"/>
       <c r="J6" s="17"/>
@@ -2755,9 +2763,9 @@
       <c r="Y6" s="23"/>
       <c r="Z6" s="23"/>
       <c r="AA6" s="23"/>
-      <c r="AT6" s="5"/>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.15">
+      <c r="AU6" s="5"/>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
         <v>14</v>
       </c>
@@ -2888,26 +2896,26 @@
         <f>'[3]Financial Model'!$Z$22</f>
         <v>0.74515549935622039</v>
       </c>
-      <c r="AO7" s="5">
+      <c r="AP7" s="5">
         <f>[3]Main!$C$24</f>
         <v>2008</v>
       </c>
-      <c r="AP7" s="5">
+      <c r="AQ7" s="5">
         <f>[3]Main!$C$25</f>
         <v>2016</v>
       </c>
-      <c r="AQ7" s="5" t="str">
+      <c r="AR7" s="5" t="str">
         <f>[3]Main!$C$23</f>
         <v>San Francisco, CA</v>
       </c>
-      <c r="AS7" s="5" t="s">
+      <c r="AT7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AT7" s="5" t="s">
+      <c r="AU7" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B8" s="7"/>
       <c r="F8" s="16"/>
       <c r="G8" s="17"/>
@@ -2933,9 +2941,9 @@
       <c r="AD8" s="18"/>
       <c r="AE8" s="18"/>
       <c r="AF8" s="18"/>
-      <c r="AT8" s="5"/>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.15">
+      <c r="AU8" s="5"/>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2954,14 +2962,14 @@
       <c r="Y9" s="23"/>
       <c r="Z9" s="23"/>
       <c r="AA9" s="23"/>
-      <c r="AS9" s="5" t="s">
+      <c r="AT9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AT9" s="5" t="s">
+      <c r="AU9" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>41</v>
       </c>
@@ -2976,14 +2984,14 @@
       <c r="Y10" s="23"/>
       <c r="Z10" s="23"/>
       <c r="AA10" s="23"/>
-      <c r="AS10" s="5" t="s">
+      <c r="AT10" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AT10" s="5" t="s">
+      <c r="AU10" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B11" s="7" t="s">
         <v>9</v>
       </c>
@@ -3114,32 +3122,32 @@
         <f>'[4]Financial Model'!$S$22</f>
         <v>4.8754062838569867E-2</v>
       </c>
-      <c r="AO11" s="5">
+      <c r="AP11" s="5">
         <f>[4]Main!$C$24</f>
         <v>1981</v>
       </c>
-      <c r="AP11" s="5">
+      <c r="AQ11" s="5">
         <f>[4]Main!$C$25</f>
         <v>1989</v>
       </c>
-      <c r="AQ11" s="5" t="str">
+      <c r="AR11" s="5" t="str">
         <f>[4]Main!$C$23</f>
         <v>Newcastle, UK</v>
       </c>
-      <c r="AS11" s="5" t="s">
+      <c r="AT11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AT11" s="5" t="s">
+      <c r="AU11" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="F12" s="16"/>
       <c r="W12" s="22"/>
-      <c r="AT12" s="5"/>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.15">
+      <c r="AU12" s="5"/>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>76</v>
       </c>
@@ -3153,27 +3161,27 @@
         <v>17</v>
       </c>
       <c r="W13" s="22"/>
-      <c r="AO13" s="5">
+      <c r="AP13" s="5">
         <v>2002</v>
       </c>
-      <c r="AP13" s="5">
+      <c r="AQ13" s="5">
         <v>2015</v>
       </c>
-      <c r="AQ13" s="5" t="str">
+      <c r="AR13" s="5" t="str">
         <f>[3]Main!$C$23</f>
         <v>San Francisco, CA</v>
       </c>
-      <c r="AS13" s="5" t="s">
+      <c r="AT13" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="AT13" s="5" t="s">
+      <c r="AU13" s="5" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.2">
       <c r="W14" s="22"/>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>48</v>
       </c>
@@ -3187,14 +3195,14 @@
         <v>17</v>
       </c>
       <c r="W15" s="22"/>
-      <c r="AS15" s="5" t="s">
+      <c r="AT15" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AT15" s="5" t="s">
+      <c r="AU15" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
@@ -3208,20 +3216,20 @@
         <v>17</v>
       </c>
       <c r="W16" s="22"/>
-      <c r="AS16" s="5" t="s">
+      <c r="AT16" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AT16" s="5" t="s">
+      <c r="AU16" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="17" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W17" s="22"/>
     </row>
-    <row r="18" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="18" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W18" s="22"/>
     </row>
-    <row r="19" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="19" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>57</v>
       </c>
@@ -3336,26 +3344,30 @@
         <f>'[5]Financial Model'!$W$28</f>
         <v>1.0772942519902369</v>
       </c>
-      <c r="AO19" s="5">
+      <c r="AO19" s="39">
+        <f>[5]Main!$G$10</f>
+        <v>2128</v>
+      </c>
+      <c r="AP19" s="5">
         <f>[5]Main!$G$8</f>
         <v>2004</v>
       </c>
-      <c r="AP19" s="5">
+      <c r="AQ19" s="5">
         <f>[5]Main!$G$7</f>
         <v>2021</v>
       </c>
-      <c r="AQ19" s="5" t="str">
+      <c r="AR19" s="5" t="str">
         <f>[5]Main!$G$6</f>
         <v>San Mateo, CA</v>
       </c>
-      <c r="AS19" s="5" t="s">
+      <c r="AT19" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AT19" s="5" t="s">
+      <c r="AU19" s="5" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="20" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>56</v>
       </c>
@@ -3397,17 +3409,17 @@
         <v>0</v>
       </c>
       <c r="W20" s="22"/>
-      <c r="AS20" s="5" t="s">
+      <c r="AT20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AT20" s="5" t="s">
+      <c r="AU20" s="5" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="21" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W21" s="22"/>
     </row>
-    <row r="22" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="22" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>87</v>
       </c>
@@ -3516,26 +3528,26 @@
         <f>'[7]Financial Model'!$AB$24</f>
         <v>0.57428577182862139</v>
       </c>
-      <c r="AO22" s="5">
+      <c r="AP22" s="5">
         <f>[7]Main!$C$24</f>
         <v>2004</v>
       </c>
-      <c r="AP22" s="5">
+      <c r="AQ22" s="5">
         <f>[7]Main!$C$25</f>
         <v>2015</v>
       </c>
-      <c r="AQ22" s="5" t="str">
+      <c r="AR22" s="5" t="str">
         <f>[7]Main!$C$23</f>
         <v>Ottowa, Canada</v>
       </c>
-      <c r="AS22" s="5" t="s">
+      <c r="AT22" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT22" s="5" t="s">
+      <c r="AU22" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="23" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B23" s="7" t="s">
         <v>82</v>
       </c>
@@ -3568,25 +3580,25 @@
         <f>[8]Main!$C$12*F57</f>
         <v>23759.870500000001</v>
       </c>
-      <c r="K23" s="37" t="str">
+      <c r="K23" s="34" t="str">
         <f>[8]Main!$C$28</f>
         <v>Q422</v>
       </c>
-      <c r="L23" s="38">
+      <c r="L23" s="35">
         <f>[8]Main!$D$28</f>
         <v>44593</v>
       </c>
       <c r="M23" s="26">
         <f>'[8]Financial Model'!$AW$29*$F$57</f>
-        <v>48.977302295869407</v>
+        <v>44.140737621104712</v>
       </c>
       <c r="N23" s="31">
         <f>'[8]Financial Model'!$AW$31</f>
-        <v>0.30118628328182151</v>
+        <v>0.17269264810788143</v>
       </c>
       <c r="O23" s="31">
         <f>'[8]Financial Model'!$AW$25</f>
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="P23" s="8"/>
       <c r="Q23" s="21">
@@ -3670,26 +3682,26 @@
         <f>'[8]Financial Model'!$AF$24</f>
         <v>8.2502266545784186E-2</v>
       </c>
-      <c r="AO23" s="5">
+      <c r="AP23" s="5">
         <f>[8]Main!$C$24</f>
         <v>1995</v>
       </c>
-      <c r="AP23" s="5">
+      <c r="AQ23" s="5">
         <f>[8]Main!$C$25</f>
         <v>1998</v>
       </c>
-      <c r="AQ23" s="5" t="str">
+      <c r="AR23" s="5" t="str">
         <f>[8]Main!$C$23</f>
         <v>San Jose, CA</v>
       </c>
-      <c r="AS23" s="5" t="s">
+      <c r="AT23" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT23" s="5" t="s">
+      <c r="AU23" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="24" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>83</v>
       </c>
@@ -3703,14 +3715,14 @@
         <v>17</v>
       </c>
       <c r="W24" s="22"/>
-      <c r="AS24" s="5" t="s">
+      <c r="AT24" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT24" s="5" t="s">
+      <c r="AU24" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="25" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="25" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>89</v>
       </c>
@@ -3724,12 +3736,12 @@
         <v>17</v>
       </c>
       <c r="W25" s="22"/>
-      <c r="AS25" s="5" t="s">
+      <c r="AT25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT25" s="5"/>
-    </row>
-    <row r="26" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU25" s="5"/>
+    </row>
+    <row r="26" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
         <v>91</v>
       </c>
@@ -3740,12 +3752,12 @@
         <v>30</v>
       </c>
       <c r="W26" s="22"/>
-      <c r="AS26" s="5" t="s">
+      <c r="AT26" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT26" s="5"/>
-    </row>
-    <row r="27" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU26" s="5"/>
+    </row>
+    <row r="27" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
         <v>93</v>
       </c>
@@ -3756,15 +3768,15 @@
         <v>33</v>
       </c>
       <c r="W27" s="22"/>
-      <c r="AT27" s="5"/>
-    </row>
-    <row r="28" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU27" s="5"/>
+    </row>
+    <row r="28" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W28" s="22"/>
     </row>
-    <row r="29" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="29" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W29" s="22"/>
     </row>
-    <row r="30" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="30" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
         <v>66</v>
       </c>
@@ -3778,11 +3790,11 @@
         <v>16</v>
       </c>
       <c r="W30" s="22"/>
-      <c r="AS30" s="5" t="s">
+      <c r="AT30" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="31" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="31" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>68</v>
       </c>
@@ -3796,17 +3808,17 @@
         <v>17</v>
       </c>
       <c r="W31" s="22"/>
-      <c r="AS31" s="5" t="s">
+      <c r="AT31" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="32" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W32" s="22"/>
     </row>
-    <row r="33" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W33" s="22"/>
     </row>
-    <row r="34" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
         <v>106</v>
       </c>
@@ -3817,14 +3829,14 @@
         <v>30</v>
       </c>
       <c r="W34" s="22"/>
-      <c r="AS34" s="5" t="s">
+      <c r="AT34" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT34" s="5" t="s">
+      <c r="AU34" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
         <v>108</v>
       </c>
@@ -3841,14 +3853,14 @@
         <v>119</v>
       </c>
       <c r="W35" s="22"/>
-      <c r="AS35" s="5" t="s">
+      <c r="AT35" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT35" s="5" t="s">
+      <c r="AU35" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
         <v>110</v>
       </c>
@@ -3859,20 +3871,20 @@
         <v>30</v>
       </c>
       <c r="W36" s="22"/>
-      <c r="AS36" s="5" t="s">
+      <c r="AT36" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="AT36" s="5" t="s">
+      <c r="AU36" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="37" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W37" s="22"/>
     </row>
-    <row r="38" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:47" x14ac:dyDescent="0.2">
       <c r="W38" s="22"/>
     </row>
-    <row r="39" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>113</v>
       </c>
@@ -3896,35 +3908,35 @@
         <v>482.83839999999998</v>
       </c>
       <c r="W39" s="22"/>
-      <c r="AO39" s="5">
+      <c r="AP39" s="5">
         <v>2007</v>
       </c>
-      <c r="AP39" s="5">
+      <c r="AQ39" s="5">
         <v>2021</v>
       </c>
-      <c r="AQ39" s="5" t="s">
+      <c r="AR39" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AS39" s="5" t="s">
+      <c r="AT39" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AT39" s="5" t="s">
+      <c r="AU39" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="40" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="40" spans="2:47" x14ac:dyDescent="0.2">
       <c r="G40" s="19"/>
       <c r="H40" s="17"/>
       <c r="W40" s="22"/>
-      <c r="AT40" s="5"/>
-    </row>
-    <row r="41" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU40" s="5"/>
+    </row>
+    <row r="41" spans="2:47" x14ac:dyDescent="0.2">
       <c r="G41" s="19"/>
       <c r="H41" s="17"/>
       <c r="W41" s="22"/>
-      <c r="AT41" s="5"/>
-    </row>
-    <row r="42" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU41" s="5"/>
+    </row>
+    <row r="42" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
         <v>121</v>
       </c>
@@ -3949,14 +3961,14 @@
         <v>122932.59181199998</v>
       </c>
       <c r="W42" s="22"/>
-      <c r="AS42" s="5" t="s">
+      <c r="AT42" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AT42" s="5" t="s">
+      <c r="AU42" s="5" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="43" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
         <v>120</v>
       </c>
@@ -3981,14 +3993,14 @@
         <v>14757.024674</v>
       </c>
       <c r="W43" s="22"/>
-      <c r="AS43" s="5" t="s">
+      <c r="AT43" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="AT43" s="5" t="s">
+      <c r="AU43" s="5" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="44" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="44" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
         <v>133</v>
       </c>
@@ -4012,20 +4024,20 @@
         <v>65.118500000000012</v>
       </c>
       <c r="W44" s="22"/>
-      <c r="AS44" s="5" t="s">
+      <c r="AT44" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="AT44" s="5" t="s">
+      <c r="AU44" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="45" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:47" x14ac:dyDescent="0.2">
       <c r="G45" s="19"/>
       <c r="H45" s="17"/>
       <c r="W45" s="22"/>
-      <c r="AT45" s="5"/>
-    </row>
-    <row r="46" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU45" s="5"/>
+    </row>
+    <row r="46" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>130</v>
       </c>
@@ -4035,9 +4047,9 @@
       <c r="G46" s="19"/>
       <c r="H46" s="17"/>
       <c r="W46" s="22"/>
-      <c r="AT46" s="5"/>
-    </row>
-    <row r="47" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU46" s="5"/>
+    </row>
+    <row r="47" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
         <v>131</v>
       </c>
@@ -4047,9 +4059,9 @@
       <c r="G47" s="19"/>
       <c r="H47" s="17"/>
       <c r="W47" s="22"/>
-      <c r="AT47" s="5"/>
-    </row>
-    <row r="48" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU47" s="5"/>
+    </row>
+    <row r="48" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
         <v>132</v>
       </c>
@@ -4059,21 +4071,21 @@
       <c r="G48" s="19"/>
       <c r="H48" s="17"/>
       <c r="W48" s="22"/>
-      <c r="AT48" s="5"/>
-    </row>
-    <row r="49" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU48" s="5"/>
+    </row>
+    <row r="49" spans="2:47" x14ac:dyDescent="0.2">
       <c r="G49" s="19"/>
       <c r="H49" s="17"/>
       <c r="W49" s="22"/>
-      <c r="AT49" s="5"/>
-    </row>
-    <row r="50" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU49" s="5"/>
+    </row>
+    <row r="50" spans="2:47" x14ac:dyDescent="0.2">
       <c r="G50" s="19"/>
       <c r="H50" s="17"/>
       <c r="W50" s="22"/>
-      <c r="AT50" s="5"/>
-    </row>
-    <row r="51" spans="2:46" x14ac:dyDescent="0.15">
+      <c r="AU50" s="5"/>
+    </row>
+    <row r="51" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B51" s="7" t="s">
         <v>150</v>
       </c>
@@ -4115,26 +4127,26 @@
         <v>0</v>
       </c>
       <c r="W51" s="22"/>
-      <c r="AO51" s="5">
+      <c r="AP51" s="5">
         <f>[9]Main!$C$24</f>
         <v>1975</v>
       </c>
-      <c r="AP51" s="5">
+      <c r="AQ51" s="5">
         <f>[9]Main!$C$25</f>
         <v>1986</v>
       </c>
-      <c r="AQ51" s="5" t="str">
+      <c r="AR51" s="5" t="str">
         <f>[9]Main!$C$23</f>
         <v>Redmond, WA</v>
       </c>
-      <c r="AS51" s="5" t="s">
+      <c r="AT51" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="AT51" s="5" t="s">
+      <c r="AU51" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="52" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B52" s="7" t="s">
         <v>151</v>
       </c>
@@ -4176,63 +4188,63 @@
         <v>0</v>
       </c>
       <c r="W52" s="22"/>
-      <c r="AO52" s="5">
+      <c r="AP52" s="5">
         <f>[10]Main!$C$24</f>
         <v>1998</v>
       </c>
-      <c r="AP52" s="5">
+      <c r="AQ52" s="5">
         <f>[10]Main!$C$25</f>
         <v>2004</v>
       </c>
-      <c r="AQ52" s="5" t="str">
+      <c r="AR52" s="5" t="str">
         <f>[10]Main!$C$23</f>
         <v>Mountain View, CA</v>
       </c>
-      <c r="AS52" s="5" t="s">
+      <c r="AT52" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="AT52" s="5" t="s">
+      <c r="AU52" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
         <v>152</v>
       </c>
       <c r="E53" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AS53" s="5" t="s">
+      <c r="AT53" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="AT53" s="5" t="s">
+      <c r="AU53" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:47" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
         <v>153</v>
       </c>
       <c r="E54" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AS54" s="5" t="s">
+      <c r="AT54" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="AT54" s="5" t="s">
+      <c r="AU54" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="56" spans="2:46" x14ac:dyDescent="0.15">
-      <c r="E56" s="34" t="s">
+    <row r="56" spans="2:47" x14ac:dyDescent="0.2">
+      <c r="E56" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="F56" s="35"/>
+      <c r="F56" s="37"/>
       <c r="G56" s="9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:47" x14ac:dyDescent="0.2">
       <c r="E57" s="10" t="s">
         <v>27</v>
       </c>
@@ -4244,7 +4256,7 @@
         <v>1.2048192771084338</v>
       </c>
     </row>
-    <row r="58" spans="2:46" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:47" x14ac:dyDescent="0.2">
       <c r="E58" s="13" t="s">
         <v>28</v>
       </c>
@@ -4293,21 +4305,21 @@
       <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1640625" style="1"/>
+    <col min="1" max="1" width="4.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
     <col min="3" max="3" width="21" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="8" width="9.1640625" style="1"/>
+    <col min="4" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.1640625" style="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -4340,7 +4352,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>52</v>
       </c>
@@ -4366,11 +4378,11 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>

</xml_diff>

<commit_message>
Create Retailers Overview sheet
</commit_message>
<xml_diff>
--- a/Overview - Software.xlsx
+++ b/Overview - Software.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20401"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\Google Drive\Stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F58C29DF-06E8-4204-A6D3-4C7006C25BC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF50572-AD06-45DB-B0E9-D5C70E59DDCC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="495" windowWidth="33600" windowHeight="18825" activeTab="1" xr2:uid="{034066B2-28C3-4551-8F6C-62966FA785BB}"/>
   </bookViews>
@@ -1040,7 +1040,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="2"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1589,12 +1589,13 @@
       <sheetName val="Main"/>
       <sheetName val="Financial Model"/>
       <sheetName val="Metrics"/>
+      <sheetName val="Earnings Call Notes"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0">
         <row r="6">
           <cell r="C6">
-            <v>33.409999999999997</v>
+            <v>30.01</v>
           </cell>
           <cell r="G6" t="str">
             <v>San Mateo, CA</v>
@@ -1602,7 +1603,7 @@
         </row>
         <row r="7">
           <cell r="C7">
-            <v>606.63699999999994</v>
+            <v>612.68899999999996</v>
           </cell>
           <cell r="G7">
             <v>2021</v>
@@ -1610,7 +1611,7 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>20267.742169999998</v>
+            <v>18386.796890000001</v>
           </cell>
           <cell r="G8">
             <v>2004</v>
@@ -1623,59 +1624,56 @@
         </row>
         <row r="11">
           <cell r="C11">
-            <v>2102.6120000000001</v>
+            <v>2020.4279999999999</v>
           </cell>
           <cell r="G11" t="str">
-            <v>Q123</v>
+            <v>Q223</v>
           </cell>
           <cell r="H11">
-            <v>40299</v>
+            <v>40026</v>
           </cell>
         </row>
         <row r="12">
           <cell r="C12">
-            <v>18165.13017</v>
+            <v>16366.368890000002</v>
           </cell>
         </row>
         <row r="16">
           <cell r="G16">
-            <v>82.664070649558042</v>
+            <v>111.9780565773442</v>
           </cell>
         </row>
         <row r="17">
           <cell r="G17">
-            <v>8.6493709068810904</v>
+            <v>7.5578091811933561</v>
           </cell>
         </row>
         <row r="18">
           <cell r="G18">
-            <v>-19.243065324183306</v>
+            <v>-15.801046113854976</v>
           </cell>
         </row>
         <row r="19">
           <cell r="G19">
-            <v>7.7520696234565314</v>
+            <v>6.7273214469950737</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="1">
         <row r="18">
-          <cell r="Y18">
+          <cell r="Z18">
             <v>-260.81599999999992</v>
           </cell>
-          <cell r="Z18">
+          <cell r="AA18">
             <v>-503.48999999999995</v>
-          </cell>
-          <cell r="AA18">
-            <v>-934.68300000000011</v>
           </cell>
         </row>
         <row r="22">
           <cell r="O22">
             <v>0.76830336433994972</v>
           </cell>
-          <cell r="AS22">
-            <v>0.09</v>
+          <cell r="AS22" t="str">
+            <v>Discount Rate</v>
           </cell>
         </row>
         <row r="23">
@@ -1694,26 +1692,25 @@
           </cell>
         </row>
         <row r="26">
-          <cell r="AS26">
-            <v>62.602343431050087</v>
+          <cell r="AS26" t="str">
+            <v>Per Share</v>
           </cell>
         </row>
         <row r="28">
           <cell r="O28">
             <v>0.22007543741412761</v>
           </cell>
-          <cell r="Z28">
+          <cell r="Z28"/>
+          <cell r="AA28">
             <v>1.0772942519902369</v>
           </cell>
-          <cell r="AA28">
-            <v>0.15937579623808262</v>
-          </cell>
-          <cell r="AS28">
-            <v>0.87376065342861708</v>
+          <cell r="AS28" t="str">
+            <v>Projected Upside</v>
           </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -2521,7 +2518,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1:J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3453,71 +3450,71 @@
       </c>
       <c r="F19" s="17">
         <f>[5]Main!$C$6*F61</f>
-        <v>27.730299999999996</v>
+        <v>24.908300000000001</v>
       </c>
       <c r="G19" s="17">
         <f>[5]Main!$C$7</f>
-        <v>606.63699999999994</v>
+        <v>612.68899999999996</v>
       </c>
       <c r="H19" s="17">
         <f>[5]Main!$C$8*F61</f>
-        <v>16822.226001099996</v>
+        <v>15261.041418700001</v>
       </c>
       <c r="I19" s="17">
         <f>[5]Main!$C$11*F61</f>
-        <v>1745.16796</v>
+        <v>1676.9552399999998</v>
       </c>
       <c r="J19" s="17">
         <f>[5]Main!$C$12*F61</f>
-        <v>15077.058041099999</v>
+        <v>13584.086178700001</v>
       </c>
       <c r="K19" s="5" t="str">
         <f>[5]Main!$G$11</f>
-        <v>Q123</v>
+        <v>Q223</v>
       </c>
       <c r="L19" s="8">
         <f>[5]Main!$H$11</f>
-        <v>40299</v>
-      </c>
-      <c r="M19" s="26">
+        <v>40026</v>
+      </c>
+      <c r="M19" s="26" t="e">
         <f>'[5]Financial Model'!$AS$26*F61</f>
-        <v>51.959945047771569</v>
-      </c>
-      <c r="N19" s="31">
+        <v>#VALUE!</v>
+      </c>
+      <c r="N19" s="31" t="str">
         <f>'[5]Financial Model'!$AS$28</f>
-        <v>0.87376065342861708</v>
-      </c>
-      <c r="O19" s="31">
+        <v>Projected Upside</v>
+      </c>
+      <c r="O19" s="31" t="str">
         <f>'[5]Financial Model'!$AS$22</f>
-        <v>0.09</v>
+        <v>Discount Rate</v>
       </c>
       <c r="Q19" s="21">
         <f>[5]Main!$G$16</f>
-        <v>82.664070649558042</v>
+        <v>111.9780565773442</v>
       </c>
       <c r="R19" s="21">
         <f>[5]Main!$G$17</f>
-        <v>8.6493709068810904</v>
+        <v>7.5578091811933561</v>
       </c>
       <c r="S19" s="21">
         <f>[5]Main!$G$19</f>
-        <v>7.7520696234565314</v>
+        <v>6.7273214469950737</v>
       </c>
       <c r="T19" s="21">
         <f>[5]Main!$G$18</f>
-        <v>-19.243065324183306</v>
+        <v>-15.801046113854976</v>
       </c>
       <c r="W19" s="23">
         <f>'[5]Financial Model'!$AA$18*F61</f>
-        <v>-775.78689000000008</v>
+        <v>-417.89669999999995</v>
       </c>
       <c r="X19" s="24">
         <f>'[5]Financial Model'!$Z$18*F61</f>
-        <v>-417.89669999999995</v>
+        <v>-216.47727999999992</v>
       </c>
       <c r="Y19" s="24">
         <f>'[5]Financial Model'!$Y$18*F61</f>
-        <v>-216.47727999999992</v>
+        <v>0</v>
       </c>
       <c r="Z19" s="22" t="s">
         <v>139</v>
@@ -3547,11 +3544,11 @@
       </c>
       <c r="AI19" s="18">
         <f>'[5]Financial Model'!$AA$28</f>
-        <v>0.15937579623808262</v>
+        <v>1.0772942519902369</v>
       </c>
       <c r="AJ19" s="18">
         <f>'[5]Financial Model'!$Z$28</f>
-        <v>1.0772942519902369</v>
+        <v>0</v>
       </c>
       <c r="AK19" s="18" t="s">
         <v>139</v>

</xml_diff>